<commit_message>
chore(docs): added some reqs and ate almost all of the PoC questions
</commit_message>
<xml_diff>
--- a/Docs/RF y RN.xlsx
+++ b/Docs/RF y RN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hecto\OneDrive\Escritorio\Personal\iroFactory\21.Mapo\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B700D17-9093-41E7-8179-4E5FEFC67B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94880F9-1816-40BA-B8C6-9A74E11E1DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,12 +18,25 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'RF-RNF'!$A$2:$I$302</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="90">
   <si>
     <t>RF</t>
   </si>
@@ -194,6 +207,105 @@
   </si>
   <si>
     <t>Y teoría de autómatas o_O (finitos y deterministas de preferencia)</t>
+  </si>
+  <si>
+    <t>Servidor</t>
+  </si>
+  <si>
+    <t>Ah we me falta hacer un diagrama para este rollo</t>
+  </si>
+  <si>
+    <t>La comunicación con entornos locales (por ejemplo, notebooks o sistemas de análisis) debe realizarse mediante una API RESTful</t>
+  </si>
+  <si>
+    <t>Backend</t>
+  </si>
+  <si>
+    <t>Clustering</t>
+  </si>
+  <si>
+    <t>Logs</t>
+  </si>
+  <si>
+    <t>Persistencia de datos</t>
+  </si>
+  <si>
+    <t>Datos Geoespaciales</t>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>Angular para el frontend</t>
+  </si>
+  <si>
+    <t>Soporte para HTTPS con certificados SSL/TLS</t>
+  </si>
+  <si>
+    <t>Integración con el SCINCE</t>
+  </si>
+  <si>
+    <t>Quizá me hace falta precisión con a qué me refiero con esto, pero realmente creo que se verá una vez entendamos cómo obtener la info de ahí</t>
+  </si>
+  <si>
+    <t>Django? Flask? FastAPI?</t>
+  </si>
+  <si>
+    <t>Framework para integrar módulos de python</t>
+  </si>
+  <si>
+    <t>K-means DBSCAN/HDBSCAN, density, spectral</t>
+  </si>
+  <si>
+    <t>Registro de consultas, errores y eventos</t>
+  </si>
+  <si>
+    <t>Sistema de caché para el navegador del usuario</t>
+  </si>
+  <si>
+    <t>Sistema de cuentas (?), podríamos recabar los datos de nuestros usuarios</t>
+  </si>
+  <si>
+    <t>Nivel estado, municipio, código postal y AGEB</t>
+  </si>
+  <si>
+    <t>Soporte para almacenamiento y consulta de datos espaciales (puntos, polígonos, relaciones)</t>
+  </si>
+  <si>
+    <t>Toda la data, con excepción de las credenciales, debe estar centralizada en el servidor</t>
+  </si>
+  <si>
+    <t>La base de datos principal debe estar orientada a grafos</t>
+  </si>
+  <si>
+    <t>Similar a la herramienta del SCINCE que permite la creación de polígonos? O solo selección de kml individuales?</t>
+  </si>
+  <si>
+    <t>Meter CORS (?), esot también entra en escalabilidad</t>
+  </si>
+  <si>
+    <t>El sitio web que muestra los análisis debe hospedarse en el mismo servidor</t>
+  </si>
+  <si>
+    <t>SOLID</t>
+  </si>
+  <si>
+    <t>Deberá tener calls dedicadas, no generales</t>
+  </si>
+  <si>
+    <t>REST API</t>
+  </si>
+  <si>
+    <t>Para paquetes muy pesados se enviará la información por chunks</t>
+  </si>
+  <si>
+    <t>A menos que a alguien se le ocurra una mejor manera :C</t>
+  </si>
+  <si>
+    <t>Templates</t>
+  </si>
+  <si>
+    <t>Para distintos negocios se necesitan distintos valores arbitrarios iniciales</t>
   </si>
 </sst>
 </file>
@@ -203,7 +315,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yy"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -278,8 +390,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="57">
+  <fills count="62">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -558,12 +676,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.499984740745262"/>
-        <bgColor rgb="FF783F04"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor rgb="FFCC0000"/>
       </patternFill>
@@ -614,6 +726,42 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor rgb="FFF6B26B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor rgb="FFF6B26B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor rgb="FFF6B26B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor rgb="FFF6B26B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFFE599"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor rgb="FFFFE599"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFE599"/>
       </patternFill>
     </fill>
   </fills>
@@ -666,7 +814,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -696,14 +844,8 @@
     <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -724,22 +866,16 @@
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -748,82 +884,67 @@
     <xf numFmtId="0" fontId="2" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="48" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="49" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="50" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="50" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="53" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="54" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="55" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -853,10 +974,47 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="57" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="58" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="59" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="60" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="61" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1087,7 +1245,9 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1103,2788 +1263,2866 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9">
-        <v>45846</v>
+        <v>45848</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="83" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="91" t="s">
+      <c r="C2" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="92" t="s">
+      <c r="D2" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="92" t="s">
+      <c r="E2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="93" t="s">
+      <c r="F2" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="91" t="s">
+      <c r="G2" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="93" t="s">
+      <c r="H2" s="82" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="53">
+      <c r="A3" s="48">
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="53">
+      <c r="E3" s="48">
         <v>1</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="57" t="s">
+      <c r="G3" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="47" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="53">
+      <c r="A4" s="48">
         <v>2</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="58" t="s">
+      <c r="B4" s="50"/>
+      <c r="C4" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="52" t="s">
+      <c r="D4" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="53">
+      <c r="E4" s="48">
         <v>2</v>
       </c>
-      <c r="F4" s="54" t="s">
+      <c r="F4" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="59"/>
+      <c r="H4" s="47" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A5" s="53">
+      <c r="A5" s="48">
         <v>3</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="52" t="s">
+      <c r="D5" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="53">
+      <c r="E5" s="48">
         <v>3</v>
       </c>
-      <c r="F5" s="56" t="s">
+      <c r="F5" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="61" t="s">
+      <c r="G5" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="52" t="s">
+      <c r="H5" s="47" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="66" x14ac:dyDescent="0.25">
-      <c r="A6" s="53">
+      <c r="A6" s="48">
         <v>4</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="62" t="s">
+      <c r="C6" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="59"/>
-      <c r="E6" s="53">
+      <c r="D6" s="50"/>
+      <c r="E6" s="48">
         <v>4</v>
       </c>
-      <c r="F6" s="56" t="s">
+      <c r="F6" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="63" t="s">
+      <c r="G6" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="64" t="s">
+      <c r="H6" s="56" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="66" x14ac:dyDescent="0.25">
-      <c r="A7" s="65">
+      <c r="A7" s="57">
         <v>5</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="62" t="s">
+      <c r="C7" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="67"/>
-      <c r="E7" s="53">
+      <c r="D7" s="58"/>
+      <c r="E7" s="48">
         <v>5</v>
       </c>
-      <c r="F7" s="56" t="s">
+      <c r="F7" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="68" t="s">
+      <c r="G7" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="52" t="s">
+      <c r="H7" s="47" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="66" x14ac:dyDescent="0.25">
-      <c r="A8" s="53">
+      <c r="A8" s="48">
         <v>6</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="69" t="s">
+      <c r="C8" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="59"/>
-      <c r="E8" s="53">
+      <c r="D8" s="50"/>
+      <c r="E8" s="48">
         <v>6</v>
       </c>
-      <c r="F8" s="56" t="s">
+      <c r="F8" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="68" t="s">
+      <c r="G8" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="59"/>
+      <c r="H8" s="50"/>
     </row>
     <row r="9" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="53">
+      <c r="A9" s="48">
         <v>7</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="70" t="s">
+      <c r="C9" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="59"/>
-      <c r="E9" s="53">
+      <c r="D9" s="50"/>
+      <c r="E9" s="48">
         <v>7</v>
       </c>
-      <c r="F9" s="56" t="s">
+      <c r="F9" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="71" t="s">
+      <c r="G9" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="59"/>
+      <c r="H9" s="50"/>
     </row>
     <row r="10" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="53">
+      <c r="A10" s="48">
         <v>8</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="52" t="s">
+      <c r="D10" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="53">
+      <c r="E10" s="48">
         <v>8</v>
       </c>
-      <c r="F10" s="56"/>
-      <c r="G10" s="71"/>
-      <c r="H10" s="59"/>
+      <c r="F10" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="53">
+      <c r="A11" s="48">
         <v>9</v>
       </c>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="73" t="s">
+      <c r="C11" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="59"/>
-      <c r="E11" s="53">
+      <c r="D11" s="50"/>
+      <c r="E11" s="48">
         <v>9</v>
       </c>
-      <c r="F11" s="56"/>
-      <c r="G11" s="71"/>
-      <c r="H11" s="59"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="50"/>
     </row>
     <row r="12" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="53">
+      <c r="A12" s="48">
         <v>10</v>
       </c>
-      <c r="B12" s="56" t="s">
+      <c r="B12" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="74" t="s">
+      <c r="C12" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="52" t="s">
+      <c r="D12" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="53">
+      <c r="E12" s="48">
         <v>10</v>
       </c>
-      <c r="F12" s="56"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="59"/>
-    </row>
-    <row r="13" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="65">
+      <c r="F12" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="89" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="50"/>
+    </row>
+    <row r="13" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="57">
         <v>11</v>
       </c>
-      <c r="B13" s="66" t="s">
+      <c r="B13" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="76" t="s">
+      <c r="C13" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="52" t="s">
+      <c r="D13" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="53"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="59"/>
+      <c r="E13" s="48">
+        <v>11</v>
+      </c>
+      <c r="F13" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="93" t="s">
+        <v>74</v>
+      </c>
+      <c r="H13" s="47" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="53">
+      <c r="A14" s="48">
         <v>12</v>
       </c>
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="77" t="s">
+      <c r="C14" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="52" t="s">
+      <c r="D14" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="53"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="79"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="69"/>
     </row>
     <row r="15" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="53">
+      <c r="A15" s="48">
         <v>13</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="80" t="s">
+      <c r="C15" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="95"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="81"/>
-      <c r="H15" s="59"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="71"/>
+      <c r="H15" s="50"/>
     </row>
     <row r="16" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="53">
+      <c r="A16" s="48">
         <v>14</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="82" t="s">
+      <c r="C16" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="59"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="83"/>
-      <c r="H16" s="59"/>
-    </row>
-    <row r="17" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="53">
+      <c r="D16" s="50"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="50"/>
+    </row>
+    <row r="17" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A17" s="48">
         <v>15</v>
       </c>
-      <c r="B17" s="56"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="83"/>
-      <c r="H17" s="59"/>
-    </row>
-    <row r="18" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="53">
+      <c r="B17" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="85" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="48"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="73"/>
+      <c r="H17" s="50"/>
+    </row>
+    <row r="18" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A18" s="48">
         <v>16</v>
       </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="84"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="85"/>
-      <c r="H18" s="59"/>
-    </row>
-    <row r="19" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="65">
+      <c r="B18" s="50"/>
+      <c r="C18" s="85" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="50"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="74"/>
+      <c r="H18" s="50"/>
+    </row>
+    <row r="19" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A19" s="57">
         <v>17</v>
       </c>
-      <c r="B19" s="66"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="85"/>
-      <c r="H19" s="59"/>
-    </row>
-    <row r="20" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="53">
+      <c r="B19" s="50"/>
+      <c r="C19" s="85" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="50"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="74"/>
+      <c r="H19" s="50"/>
+    </row>
+    <row r="20" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A20" s="48">
         <v>18</v>
       </c>
-      <c r="B20" s="56"/>
-      <c r="C20" s="84"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="85"/>
-      <c r="H20" s="59"/>
-    </row>
-    <row r="21" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A21" s="53">
+      <c r="B20" s="50"/>
+      <c r="C20" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="50"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="74"/>
+      <c r="H20" s="50"/>
+    </row>
+    <row r="21" spans="1:8" ht="66" x14ac:dyDescent="0.25">
+      <c r="A21" s="48">
         <v>19</v>
       </c>
-      <c r="B21" s="56"/>
-      <c r="C21" s="84"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="85"/>
-      <c r="H21" s="59"/>
+      <c r="B21" s="87" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="86" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="48"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="50"/>
     </row>
     <row r="22" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="53">
+      <c r="A22" s="48">
         <v>20</v>
       </c>
-      <c r="B22" s="56"/>
-      <c r="C22" s="84"/>
-      <c r="D22" s="59"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="86"/>
-      <c r="H22" s="59"/>
-    </row>
-    <row r="23" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A23" s="53"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="59"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="87"/>
-      <c r="H23" s="59"/>
-    </row>
-    <row r="24" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A24" s="53"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="84"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="59"/>
+      <c r="B22" s="87"/>
+      <c r="C22" s="86" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="48"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="50"/>
+    </row>
+    <row r="23" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A23" s="48">
+        <v>21</v>
+      </c>
+      <c r="B23" s="87" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="88" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="48"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="76"/>
+      <c r="H23" s="50"/>
+    </row>
+    <row r="24" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A24" s="48">
+        <v>22</v>
+      </c>
+      <c r="B24" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="95" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="48"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="50"/>
     </row>
     <row r="25" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A25" s="53"/>
-      <c r="B25" s="56"/>
-      <c r="C25" s="84"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="88"/>
-      <c r="H25" s="59"/>
-    </row>
-    <row r="26" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A26" s="53"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="89"/>
-      <c r="D26" s="59"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="87"/>
-      <c r="H26" s="59"/>
-    </row>
-    <row r="27" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="49"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="2"/>
+      <c r="A25" s="48">
+        <v>23</v>
+      </c>
+      <c r="B25" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="90" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="48"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="77"/>
+      <c r="H25" s="50"/>
+    </row>
+    <row r="26" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A26" s="48">
+        <v>24</v>
+      </c>
+      <c r="B26" s="47"/>
+      <c r="C26" s="90" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" s="48"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="76"/>
+      <c r="H26" s="50"/>
+    </row>
+    <row r="27" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>25</v>
+      </c>
+      <c r="B27" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" s="97" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="50"/>
       <c r="E27" s="6"/>
-      <c r="F27" s="49"/>
+      <c r="F27" s="2"/>
       <c r="G27" s="21"/>
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
-      <c r="B28" s="49"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="2"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="78"/>
+      <c r="D28" s="50"/>
       <c r="E28" s="6"/>
-      <c r="F28" s="49"/>
+      <c r="F28" s="2"/>
       <c r="G28" s="21"/>
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
-      <c r="B29" s="49"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="2"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="50"/>
       <c r="E29" s="6"/>
-      <c r="F29" s="49"/>
+      <c r="F29" s="2"/>
       <c r="G29" s="14"/>
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
-      <c r="B30" s="49"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="2"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="50"/>
       <c r="E30" s="6"/>
-      <c r="F30" s="49"/>
+      <c r="F30" s="2"/>
       <c r="G30" s="14"/>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
-      <c r="B31" s="49"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="2"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="68"/>
+      <c r="D31" s="50"/>
       <c r="E31" s="6"/>
-      <c r="F31" s="49"/>
+      <c r="F31" s="2"/>
       <c r="G31" s="14"/>
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
-      <c r="B32" s="49"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="2"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="50"/>
       <c r="E32" s="6"/>
-      <c r="F32" s="49"/>
+      <c r="F32" s="2"/>
       <c r="G32" s="14"/>
       <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
-      <c r="B33" s="49"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="2"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="91"/>
+      <c r="D33" s="50"/>
       <c r="E33" s="6"/>
-      <c r="F33" s="49"/>
+      <c r="F33" s="2"/>
       <c r="G33" s="14"/>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
-      <c r="B34" s="49"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="2"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="50"/>
       <c r="E34" s="6"/>
-      <c r="F34" s="49"/>
+      <c r="F34" s="2"/>
       <c r="G34" s="22"/>
       <c r="H34" s="2"/>
       <c r="I34" s="4"/>
     </row>
     <row r="35" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
-      <c r="B35" s="49"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="2"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="94"/>
+      <c r="D35" s="50"/>
       <c r="E35" s="6"/>
-      <c r="F35" s="49"/>
+      <c r="F35" s="2"/>
       <c r="G35" s="22"/>
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
-      <c r="B36" s="49"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="2"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="50"/>
       <c r="E36" s="6"/>
-      <c r="F36" s="49"/>
+      <c r="F36" s="2"/>
       <c r="G36" s="22"/>
       <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
-      <c r="B37" s="49"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="2"/>
+      <c r="B37" s="47"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="50"/>
       <c r="E37" s="6"/>
-      <c r="F37" s="49"/>
+      <c r="F37" s="2"/>
       <c r="G37" s="22"/>
       <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
-      <c r="B38" s="49"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="2"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="50"/>
       <c r="E38" s="6"/>
-      <c r="F38" s="49"/>
+      <c r="F38" s="2"/>
       <c r="G38" s="22"/>
       <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
-      <c r="B39" s="49"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="2"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="92"/>
+      <c r="D39" s="50"/>
       <c r="E39" s="6"/>
-      <c r="F39" s="49"/>
+      <c r="F39" s="2"/>
       <c r="G39" s="23"/>
       <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
-      <c r="B40" s="49"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="2"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="92"/>
+      <c r="D40" s="50"/>
       <c r="E40" s="6"/>
-      <c r="F40" s="49"/>
+      <c r="F40" s="2"/>
       <c r="G40" s="23"/>
       <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
-      <c r="B41" s="49"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="2"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="92"/>
+      <c r="D41" s="50"/>
       <c r="E41" s="6"/>
-      <c r="F41" s="49"/>
+      <c r="F41" s="2"/>
       <c r="G41" s="23"/>
       <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
-      <c r="B42" s="49"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="2"/>
+      <c r="B42" s="50"/>
+      <c r="C42" s="92"/>
+      <c r="D42" s="50"/>
       <c r="E42" s="6"/>
-      <c r="F42" s="49"/>
+      <c r="F42" s="2"/>
       <c r="G42" s="23"/>
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
-      <c r="B43" s="49"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="2"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="92"/>
+      <c r="D43" s="50"/>
       <c r="E43" s="6"/>
-      <c r="F43" s="49"/>
+      <c r="F43" s="2"/>
       <c r="G43" s="23"/>
       <c r="H43" s="2"/>
     </row>
     <row r="44" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
-      <c r="B44" s="49"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="2"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="92"/>
+      <c r="D44" s="50"/>
       <c r="E44" s="6"/>
-      <c r="F44" s="49"/>
+      <c r="F44" s="2"/>
       <c r="G44" s="23"/>
       <c r="H44" s="2"/>
     </row>
     <row r="45" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
-      <c r="B45" s="49"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="2"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="50"/>
       <c r="E45" s="6"/>
-      <c r="F45" s="49"/>
+      <c r="F45" s="2"/>
       <c r="G45" s="23"/>
       <c r="H45" s="2"/>
     </row>
     <row r="46" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
-      <c r="B46" s="49"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="50"/>
       <c r="E46" s="6"/>
-      <c r="F46" s="49"/>
+      <c r="F46" s="2"/>
       <c r="G46" s="23"/>
       <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
-      <c r="B47" s="49"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="50"/>
       <c r="E47" s="6"/>
-      <c r="F47" s="49"/>
+      <c r="F47" s="2"/>
       <c r="G47" s="23"/>
       <c r="H47" s="2"/>
     </row>
     <row r="48" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
-      <c r="B48" s="49"/>
-      <c r="C48" s="28"/>
-      <c r="D48" s="2"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="50"/>
       <c r="E48" s="6"/>
-      <c r="F48" s="49"/>
+      <c r="F48" s="2"/>
       <c r="G48" s="23"/>
       <c r="H48" s="2"/>
     </row>
     <row r="49" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
-      <c r="B49" s="49"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="96"/>
+      <c r="D49" s="50"/>
       <c r="E49" s="6"/>
-      <c r="F49" s="49"/>
+      <c r="F49" s="2"/>
       <c r="G49" s="23"/>
       <c r="H49" s="2"/>
     </row>
     <row r="50" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
-      <c r="B50" s="49"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="50"/>
       <c r="E50" s="6"/>
-      <c r="F50" s="49"/>
+      <c r="F50" s="2"/>
       <c r="G50" s="24"/>
       <c r="H50" s="2"/>
     </row>
     <row r="51" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
-      <c r="B51" s="49"/>
-      <c r="C51" s="28"/>
-      <c r="D51" s="2"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="50"/>
       <c r="E51" s="6"/>
-      <c r="F51" s="49"/>
+      <c r="F51" s="2"/>
       <c r="G51" s="24"/>
       <c r="H51" s="2"/>
     </row>
     <row r="52" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
-      <c r="B52" s="49"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="96"/>
+      <c r="D52" s="50"/>
       <c r="E52" s="6"/>
-      <c r="F52" s="49"/>
+      <c r="F52" s="2"/>
       <c r="G52" s="24"/>
       <c r="H52" s="2"/>
     </row>
     <row r="53" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
-      <c r="B53" s="49"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="50"/>
       <c r="E53" s="6"/>
-      <c r="F53" s="49"/>
+      <c r="F53" s="2"/>
       <c r="G53" s="24"/>
       <c r="H53" s="2"/>
     </row>
     <row r="54" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
-      <c r="B54" s="49"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="50"/>
       <c r="E54" s="6"/>
-      <c r="F54" s="49"/>
+      <c r="F54" s="2"/>
       <c r="G54" s="24"/>
       <c r="H54" s="2"/>
     </row>
     <row r="55" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
-      <c r="B55" s="49"/>
-      <c r="C55" s="29"/>
-      <c r="D55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="50"/>
       <c r="E55" s="6"/>
-      <c r="F55" s="49"/>
+      <c r="F55" s="2"/>
       <c r="G55" s="24"/>
       <c r="H55" s="2"/>
     </row>
     <row r="56" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
-      <c r="B56" s="49"/>
-      <c r="C56" s="29"/>
-      <c r="D56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="50"/>
       <c r="E56" s="6"/>
-      <c r="F56" s="49"/>
+      <c r="F56" s="2"/>
       <c r="G56" s="24"/>
       <c r="H56" s="2"/>
     </row>
     <row r="57" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
-      <c r="B57" s="49"/>
-      <c r="C57" s="29"/>
-      <c r="D57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="50"/>
       <c r="E57" s="6"/>
-      <c r="F57" s="49"/>
+      <c r="F57" s="2"/>
       <c r="G57" s="24"/>
       <c r="H57" s="2"/>
     </row>
     <row r="58" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
-      <c r="B58" s="49"/>
-      <c r="C58" s="15"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="20"/>
       <c r="D58" s="2"/>
       <c r="E58" s="6"/>
-      <c r="F58" s="49"/>
+      <c r="F58" s="2"/>
       <c r="G58" s="24"/>
       <c r="H58" s="2"/>
     </row>
     <row r="59" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
-      <c r="B59" s="49"/>
-      <c r="C59" s="15"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="20"/>
       <c r="D59" s="2"/>
       <c r="E59" s="6"/>
-      <c r="F59" s="49"/>
+      <c r="F59" s="2"/>
       <c r="G59" s="24"/>
       <c r="H59" s="2"/>
     </row>
     <row r="60" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
-      <c r="B60" s="49"/>
-      <c r="C60" s="15"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="20"/>
       <c r="D60" s="2"/>
       <c r="E60" s="6"/>
-      <c r="F60" s="49"/>
+      <c r="F60" s="2"/>
       <c r="G60" s="24"/>
       <c r="H60" s="2"/>
     </row>
     <row r="61" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
-      <c r="B61" s="49"/>
-      <c r="C61" s="24"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="20"/>
       <c r="D61" s="2"/>
       <c r="E61" s="6"/>
-      <c r="F61" s="49"/>
+      <c r="F61" s="2"/>
       <c r="G61" s="24"/>
       <c r="H61" s="2"/>
     </row>
     <row r="62" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
-      <c r="B62" s="49"/>
-      <c r="C62" s="19"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="20"/>
       <c r="D62" s="2"/>
       <c r="E62" s="6"/>
-      <c r="F62" s="49"/>
+      <c r="F62" s="2"/>
       <c r="G62" s="24"/>
       <c r="H62" s="2"/>
     </row>
     <row r="63" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
-      <c r="B63" s="49"/>
-      <c r="C63" s="19"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="20"/>
       <c r="D63" s="2"/>
       <c r="E63" s="6"/>
-      <c r="F63" s="49"/>
+      <c r="F63" s="2"/>
       <c r="G63" s="24"/>
       <c r="H63" s="2"/>
     </row>
     <row r="64" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
-      <c r="B64" s="49"/>
-      <c r="C64" s="19"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="20"/>
       <c r="D64" s="2"/>
       <c r="E64" s="6"/>
-      <c r="F64" s="49"/>
+      <c r="F64" s="2"/>
       <c r="G64" s="24"/>
       <c r="H64" s="2"/>
     </row>
     <row r="65" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
-      <c r="B65" s="49"/>
-      <c r="C65" s="19"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="20"/>
       <c r="D65" s="2"/>
       <c r="E65" s="6"/>
-      <c r="F65" s="49"/>
+      <c r="F65" s="2"/>
       <c r="G65" s="25"/>
       <c r="H65" s="2"/>
     </row>
     <row r="66" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
-      <c r="B66" s="49"/>
+      <c r="B66" s="2"/>
       <c r="C66" s="20"/>
       <c r="D66" s="2"/>
       <c r="E66" s="6"/>
-      <c r="F66" s="49"/>
+      <c r="F66" s="2"/>
       <c r="G66" s="25"/>
       <c r="H66" s="2"/>
     </row>
     <row r="67" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
-      <c r="B67" s="49"/>
+      <c r="B67" s="2"/>
       <c r="C67" s="20"/>
       <c r="D67" s="2"/>
       <c r="E67" s="6"/>
-      <c r="F67" s="49"/>
+      <c r="F67" s="2"/>
       <c r="G67" s="25"/>
       <c r="H67" s="2"/>
     </row>
     <row r="68" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
-      <c r="B68" s="49"/>
+      <c r="B68" s="2"/>
       <c r="C68" s="20"/>
       <c r="D68" s="2"/>
       <c r="E68" s="6"/>
-      <c r="F68" s="49"/>
+      <c r="F68" s="2"/>
       <c r="G68" s="26"/>
       <c r="H68" s="2"/>
     </row>
     <row r="69" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
-      <c r="B69" s="49"/>
+      <c r="B69" s="2"/>
       <c r="C69" s="20"/>
       <c r="D69" s="2"/>
       <c r="E69" s="6"/>
-      <c r="F69" s="49"/>
+      <c r="F69" s="2"/>
       <c r="G69" s="26"/>
       <c r="H69" s="2"/>
     </row>
     <row r="70" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
-      <c r="B70" s="49"/>
-      <c r="C70" s="30"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="20"/>
       <c r="D70" s="2"/>
       <c r="E70" s="6"/>
-      <c r="F70" s="49"/>
+      <c r="F70" s="2"/>
       <c r="G70" s="26"/>
       <c r="H70" s="2"/>
     </row>
     <row r="71" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
-      <c r="B71" s="49"/>
-      <c r="C71" s="31"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="20"/>
       <c r="D71" s="2"/>
       <c r="E71" s="6"/>
-      <c r="F71" s="49"/>
+      <c r="F71" s="2"/>
       <c r="G71" s="26"/>
       <c r="H71" s="2"/>
     </row>
     <row r="72" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="6"/>
-      <c r="B72" s="49"/>
-      <c r="C72" s="31"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="20"/>
       <c r="D72" s="2"/>
       <c r="E72" s="6"/>
-      <c r="F72" s="49"/>
+      <c r="F72" s="2"/>
       <c r="G72" s="26"/>
       <c r="H72" s="2"/>
     </row>
     <row r="73" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
-      <c r="B73" s="49"/>
-      <c r="C73" s="31"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="20"/>
       <c r="D73" s="2"/>
       <c r="E73" s="6"/>
-      <c r="F73" s="49"/>
+      <c r="F73" s="2"/>
       <c r="G73" s="26"/>
       <c r="H73" s="2"/>
     </row>
     <row r="74" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
-      <c r="B74" s="49"/>
-      <c r="C74" s="31"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="20"/>
       <c r="D74" s="2"/>
       <c r="E74" s="6"/>
-      <c r="F74" s="49"/>
+      <c r="F74" s="2"/>
       <c r="G74" s="26"/>
       <c r="H74" s="2"/>
     </row>
     <row r="75" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
-      <c r="B75" s="49"/>
-      <c r="C75" s="31"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="20"/>
       <c r="D75" s="2"/>
       <c r="E75" s="6"/>
-      <c r="F75" s="49"/>
+      <c r="F75" s="2"/>
       <c r="G75" s="26"/>
       <c r="H75" s="2"/>
     </row>
     <row r="76" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
-      <c r="B76" s="49"/>
-      <c r="C76" s="31"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="20"/>
       <c r="D76" s="2"/>
       <c r="E76" s="6"/>
-      <c r="F76" s="49"/>
+      <c r="F76" s="2"/>
       <c r="G76" s="26"/>
       <c r="H76" s="2"/>
     </row>
     <row r="77" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
-      <c r="B77" s="49"/>
-      <c r="C77" s="31"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="20"/>
       <c r="D77" s="2"/>
       <c r="E77" s="6"/>
-      <c r="F77" s="49"/>
+      <c r="F77" s="2"/>
       <c r="G77" s="26"/>
       <c r="H77" s="2"/>
     </row>
     <row r="78" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
-      <c r="B78" s="49"/>
-      <c r="C78" s="32"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="20"/>
       <c r="D78" s="2"/>
       <c r="E78" s="6"/>
-      <c r="F78" s="49"/>
-      <c r="G78" s="28"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="27"/>
       <c r="H78" s="2"/>
     </row>
     <row r="79" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
-      <c r="B79" s="49"/>
-      <c r="C79" s="32"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="20"/>
       <c r="D79" s="2"/>
       <c r="E79" s="6"/>
-      <c r="F79" s="49"/>
-      <c r="G79" s="28"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="27"/>
       <c r="H79" s="2"/>
     </row>
     <row r="80" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="6"/>
-      <c r="B80" s="49"/>
-      <c r="C80" s="32"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="20"/>
       <c r="D80" s="2"/>
       <c r="E80" s="6"/>
-      <c r="F80" s="49"/>
-      <c r="G80" s="28"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="27"/>
       <c r="H80" s="2"/>
     </row>
     <row r="81" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="6"/>
-      <c r="B81" s="49"/>
-      <c r="C81" s="32"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="20"/>
       <c r="D81" s="2"/>
       <c r="E81" s="6"/>
-      <c r="F81" s="49"/>
-      <c r="G81" s="28"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="27"/>
       <c r="H81" s="2"/>
     </row>
     <row r="82" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="6"/>
-      <c r="B82" s="49"/>
-      <c r="C82" s="33"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="20"/>
       <c r="D82" s="2"/>
       <c r="E82" s="6"/>
-      <c r="F82" s="49"/>
-      <c r="G82" s="28"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="27"/>
       <c r="H82" s="2"/>
     </row>
     <row r="83" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
-      <c r="B83" s="49"/>
-      <c r="C83" s="33"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="20"/>
       <c r="D83" s="2"/>
       <c r="E83" s="6"/>
-      <c r="F83" s="49"/>
-      <c r="G83" s="28"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="27"/>
       <c r="H83" s="2"/>
     </row>
     <row r="84" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A84" s="6"/>
-      <c r="B84" s="49"/>
-      <c r="C84" s="16"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="20"/>
       <c r="D84" s="2"/>
       <c r="E84" s="6"/>
-      <c r="F84" s="49"/>
-      <c r="G84" s="28"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="27"/>
       <c r="H84" s="2"/>
     </row>
     <row r="85" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
-      <c r="B85" s="49"/>
-      <c r="C85" s="34"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="20"/>
       <c r="D85" s="2"/>
       <c r="E85" s="6"/>
-      <c r="F85" s="49"/>
-      <c r="G85" s="28"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="27"/>
       <c r="H85" s="2"/>
     </row>
     <row r="86" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A86" s="6"/>
-      <c r="B86" s="49"/>
-      <c r="C86" s="34"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="20"/>
       <c r="D86" s="2"/>
       <c r="E86" s="6"/>
-      <c r="F86" s="49"/>
-      <c r="G86" s="29"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="28"/>
       <c r="H86" s="2"/>
     </row>
     <row r="87" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A87" s="6"/>
-      <c r="B87" s="49"/>
-      <c r="C87" s="35"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="20"/>
       <c r="D87" s="2"/>
       <c r="E87" s="6"/>
-      <c r="F87" s="49"/>
-      <c r="G87" s="29"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="28"/>
       <c r="H87" s="2"/>
     </row>
     <row r="88" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A88" s="6"/>
-      <c r="B88" s="49"/>
-      <c r="C88" s="35"/>
+      <c r="B88" s="2"/>
+      <c r="C88" s="20"/>
       <c r="D88" s="2"/>
       <c r="E88" s="6"/>
-      <c r="F88" s="49"/>
-      <c r="G88" s="29"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="28"/>
       <c r="H88" s="2"/>
     </row>
     <row r="89" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A89" s="6"/>
-      <c r="B89" s="49"/>
-      <c r="C89" s="35"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="20"/>
       <c r="D89" s="2"/>
       <c r="E89" s="6"/>
-      <c r="F89" s="49"/>
-      <c r="G89" s="29"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="28"/>
       <c r="H89" s="2"/>
     </row>
     <row r="90" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A90" s="6"/>
-      <c r="B90" s="49"/>
-      <c r="C90" s="35"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="20"/>
       <c r="D90" s="2"/>
       <c r="E90" s="6"/>
-      <c r="F90" s="49"/>
-      <c r="G90" s="29"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="28"/>
       <c r="H90" s="2"/>
     </row>
     <row r="91" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A91" s="6"/>
-      <c r="B91" s="49"/>
-      <c r="C91" s="36"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="20"/>
       <c r="D91" s="2"/>
       <c r="E91" s="6"/>
-      <c r="F91" s="49"/>
-      <c r="G91" s="29"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="28"/>
       <c r="H91" s="2"/>
     </row>
     <row r="92" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
-      <c r="B92" s="49"/>
-      <c r="C92" s="36"/>
+      <c r="B92" s="2"/>
+      <c r="C92" s="20"/>
       <c r="D92" s="2"/>
       <c r="E92" s="6"/>
-      <c r="F92" s="49"/>
+      <c r="F92" s="2"/>
       <c r="G92" s="15"/>
       <c r="H92" s="2"/>
     </row>
     <row r="93" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A93" s="6"/>
-      <c r="B93" s="49"/>
-      <c r="C93" s="37"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="20"/>
       <c r="D93" s="2"/>
       <c r="E93" s="6"/>
-      <c r="F93" s="49"/>
+      <c r="F93" s="2"/>
       <c r="G93" s="15"/>
       <c r="H93" s="2"/>
     </row>
     <row r="94" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A94" s="6"/>
-      <c r="B94" s="49"/>
-      <c r="C94" s="37"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="20"/>
       <c r="D94" s="2"/>
       <c r="E94" s="6"/>
-      <c r="F94" s="49"/>
+      <c r="F94" s="2"/>
       <c r="G94" s="15"/>
       <c r="H94" s="2"/>
     </row>
     <row r="95" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A95" s="6"/>
-      <c r="B95" s="49"/>
-      <c r="C95" s="37"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="20"/>
       <c r="D95" s="2"/>
       <c r="E95" s="6"/>
-      <c r="F95" s="49"/>
+      <c r="F95" s="2"/>
       <c r="G95" s="15"/>
       <c r="H95" s="2"/>
     </row>
     <row r="96" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A96" s="6"/>
-      <c r="B96" s="49"/>
-      <c r="C96" s="37"/>
+      <c r="B96" s="2"/>
+      <c r="C96" s="20"/>
       <c r="D96" s="2"/>
       <c r="E96" s="6"/>
-      <c r="F96" s="49"/>
+      <c r="F96" s="2"/>
       <c r="G96" s="15"/>
       <c r="H96" s="2"/>
     </row>
     <row r="97" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A97" s="6"/>
-      <c r="B97" s="49"/>
-      <c r="C97" s="37"/>
+      <c r="B97" s="2"/>
+      <c r="C97" s="20"/>
       <c r="D97" s="2"/>
       <c r="E97" s="6"/>
-      <c r="F97" s="49"/>
+      <c r="F97" s="2"/>
       <c r="G97" s="15"/>
       <c r="H97" s="2"/>
     </row>
     <row r="98" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A98" s="6"/>
-      <c r="B98" s="49"/>
-      <c r="C98" s="37"/>
+      <c r="B98" s="2"/>
+      <c r="C98" s="20"/>
       <c r="D98" s="2"/>
       <c r="E98" s="6"/>
-      <c r="F98" s="49"/>
+      <c r="F98" s="2"/>
       <c r="G98" s="15"/>
       <c r="H98" s="2"/>
     </row>
     <row r="99" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A99" s="6"/>
-      <c r="B99" s="49"/>
-      <c r="C99" s="37"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="35"/>
       <c r="D99" s="2"/>
       <c r="E99" s="6"/>
-      <c r="F99" s="49"/>
+      <c r="F99" s="2"/>
       <c r="G99" s="15"/>
       <c r="H99" s="2"/>
     </row>
     <row r="100" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A100" s="6"/>
-      <c r="B100" s="49"/>
-      <c r="C100" s="38"/>
+      <c r="B100" s="2"/>
+      <c r="C100" s="36"/>
       <c r="D100" s="2"/>
       <c r="E100" s="6"/>
-      <c r="F100" s="49"/>
+      <c r="F100" s="2"/>
       <c r="G100" s="24"/>
       <c r="H100" s="2"/>
     </row>
     <row r="101" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A101" s="6"/>
-      <c r="B101" s="49"/>
-      <c r="C101" s="38"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="36"/>
       <c r="D101" s="2"/>
       <c r="E101" s="6"/>
-      <c r="F101" s="49"/>
+      <c r="F101" s="2"/>
       <c r="G101" s="24"/>
       <c r="H101" s="2"/>
     </row>
     <row r="102" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A102" s="6"/>
-      <c r="B102" s="49"/>
-      <c r="C102" s="39"/>
+      <c r="B102" s="2"/>
+      <c r="C102" s="37"/>
       <c r="D102" s="2"/>
       <c r="E102" s="6"/>
-      <c r="F102" s="49"/>
+      <c r="F102" s="2"/>
       <c r="G102" s="24"/>
       <c r="H102" s="3"/>
     </row>
     <row r="103" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A103" s="10"/>
-      <c r="B103" s="50"/>
-      <c r="C103" s="39"/>
+      <c r="B103" s="13"/>
+      <c r="C103" s="37"/>
       <c r="D103" s="3"/>
       <c r="E103" s="6"/>
-      <c r="F103" s="49"/>
+      <c r="F103" s="2"/>
       <c r="G103" s="24"/>
       <c r="H103" s="3"/>
     </row>
     <row r="104" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A104" s="6"/>
-      <c r="B104" s="49"/>
-      <c r="C104" s="39"/>
+      <c r="B104" s="2"/>
+      <c r="C104" s="37"/>
       <c r="D104" s="3"/>
       <c r="E104" s="6"/>
-      <c r="F104" s="49"/>
+      <c r="F104" s="2"/>
       <c r="G104" s="19"/>
       <c r="H104" s="3"/>
     </row>
     <row r="105" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A105" s="6"/>
-      <c r="B105" s="49"/>
-      <c r="C105" s="39"/>
+      <c r="B105" s="2"/>
+      <c r="C105" s="37"/>
       <c r="D105" s="3"/>
       <c r="E105" s="6"/>
-      <c r="F105" s="49"/>
+      <c r="F105" s="2"/>
       <c r="G105" s="19"/>
       <c r="H105" s="3"/>
     </row>
     <row r="106" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A106" s="6"/>
-      <c r="B106" s="49"/>
-      <c r="C106" s="40"/>
+      <c r="B106" s="2"/>
+      <c r="C106" s="38"/>
       <c r="D106" s="3"/>
       <c r="E106" s="6"/>
-      <c r="F106" s="49"/>
+      <c r="F106" s="2"/>
       <c r="G106" s="19"/>
       <c r="H106" s="3"/>
     </row>
     <row r="107" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A107" s="6"/>
-      <c r="B107" s="49"/>
-      <c r="C107" s="40"/>
+      <c r="B107" s="2"/>
+      <c r="C107" s="38"/>
       <c r="D107" s="3"/>
       <c r="E107" s="6"/>
-      <c r="F107" s="49"/>
-      <c r="G107" s="48"/>
+      <c r="F107" s="2"/>
+      <c r="G107" s="46"/>
       <c r="H107" s="3"/>
     </row>
     <row r="108" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A108" s="6"/>
-      <c r="B108" s="49"/>
-      <c r="C108" s="40"/>
+      <c r="B108" s="2"/>
+      <c r="C108" s="38"/>
       <c r="D108" s="3"/>
       <c r="E108" s="6"/>
-      <c r="F108" s="49"/>
+      <c r="F108" s="2"/>
       <c r="G108" s="19"/>
       <c r="H108" s="2"/>
     </row>
     <row r="109" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A109" s="6"/>
-      <c r="B109" s="49"/>
-      <c r="C109" s="40"/>
+      <c r="B109" s="2"/>
+      <c r="C109" s="38"/>
       <c r="D109" s="2"/>
       <c r="E109" s="6"/>
-      <c r="F109" s="49"/>
+      <c r="F109" s="2"/>
       <c r="G109" s="19"/>
       <c r="H109" s="2"/>
     </row>
     <row r="110" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A110" s="6"/>
-      <c r="B110" s="49"/>
+      <c r="B110" s="2"/>
       <c r="C110" s="18"/>
       <c r="D110" s="2"/>
       <c r="E110" s="6"/>
-      <c r="F110" s="49"/>
+      <c r="F110" s="2"/>
       <c r="G110" s="19"/>
       <c r="H110" s="2"/>
     </row>
     <row r="111" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A111" s="6"/>
-      <c r="B111" s="49"/>
+      <c r="B111" s="2"/>
       <c r="C111" s="13"/>
       <c r="D111" s="2"/>
       <c r="E111" s="6"/>
-      <c r="F111" s="49"/>
+      <c r="F111" s="2"/>
       <c r="G111" s="19"/>
       <c r="H111" s="2"/>
     </row>
     <row r="112" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A112" s="6"/>
-      <c r="B112" s="49"/>
+      <c r="B112" s="2"/>
       <c r="C112" s="13"/>
       <c r="D112" s="2"/>
       <c r="E112" s="6"/>
-      <c r="F112" s="49"/>
+      <c r="F112" s="2"/>
       <c r="G112" s="19"/>
       <c r="H112" s="2"/>
     </row>
     <row r="113" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A113" s="6"/>
-      <c r="B113" s="49"/>
+      <c r="B113" s="2"/>
       <c r="C113" s="13"/>
       <c r="D113" s="2"/>
       <c r="E113" s="6"/>
-      <c r="F113" s="49"/>
+      <c r="F113" s="2"/>
       <c r="G113" s="19"/>
       <c r="H113" s="2"/>
     </row>
     <row r="114" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A114" s="6"/>
-      <c r="B114" s="49"/>
+      <c r="B114" s="2"/>
       <c r="C114" s="13"/>
       <c r="D114" s="2"/>
       <c r="E114" s="6"/>
-      <c r="F114" s="49"/>
+      <c r="F114" s="2"/>
       <c r="G114" s="19"/>
       <c r="H114" s="2"/>
     </row>
     <row r="115" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A115" s="6"/>
-      <c r="B115" s="49"/>
+      <c r="B115" s="2"/>
       <c r="C115" s="13"/>
       <c r="D115" s="2"/>
       <c r="E115" s="6"/>
-      <c r="F115" s="49"/>
+      <c r="F115" s="2"/>
       <c r="G115" s="20"/>
       <c r="H115" s="8"/>
     </row>
     <row r="116" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A116" s="11"/>
-      <c r="B116" s="51"/>
+      <c r="B116" s="8"/>
       <c r="C116" s="13"/>
       <c r="D116" s="8"/>
       <c r="E116" s="6"/>
-      <c r="F116" s="49"/>
+      <c r="F116" s="2"/>
       <c r="G116" s="20"/>
       <c r="H116" s="2"/>
     </row>
     <row r="117" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A117" s="6"/>
-      <c r="B117" s="49"/>
+      <c r="B117" s="2"/>
       <c r="C117" s="13"/>
       <c r="D117" s="2"/>
       <c r="E117" s="6"/>
-      <c r="F117" s="49"/>
+      <c r="F117" s="2"/>
       <c r="G117" s="20"/>
       <c r="H117" s="2"/>
     </row>
     <row r="118" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A118" s="6"/>
-      <c r="B118" s="49"/>
+      <c r="B118" s="2"/>
       <c r="C118" s="13"/>
       <c r="D118" s="2"/>
       <c r="E118" s="6"/>
-      <c r="F118" s="49"/>
+      <c r="F118" s="2"/>
       <c r="G118" s="20"/>
       <c r="H118" s="2"/>
     </row>
     <row r="119" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A119" s="6"/>
-      <c r="B119" s="49"/>
+      <c r="B119" s="2"/>
       <c r="C119" s="13"/>
       <c r="D119" s="2"/>
       <c r="E119" s="6"/>
-      <c r="F119" s="49"/>
+      <c r="F119" s="2"/>
       <c r="G119" s="20"/>
       <c r="H119" s="2"/>
     </row>
     <row r="120" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A120" s="6"/>
-      <c r="B120" s="49"/>
+      <c r="B120" s="2"/>
       <c r="C120" s="13"/>
       <c r="D120" s="2"/>
       <c r="E120" s="6"/>
-      <c r="F120" s="49"/>
-      <c r="G120" s="31"/>
+      <c r="F120" s="2"/>
+      <c r="G120" s="29"/>
       <c r="H120" s="2"/>
     </row>
     <row r="121" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A121" s="6"/>
-      <c r="B121" s="49"/>
+      <c r="B121" s="2"/>
       <c r="C121" s="13"/>
       <c r="D121" s="2"/>
       <c r="E121" s="6"/>
-      <c r="F121" s="49"/>
-      <c r="G121" s="31"/>
+      <c r="F121" s="2"/>
+      <c r="G121" s="29"/>
       <c r="H121" s="2"/>
     </row>
     <row r="122" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A122" s="6"/>
-      <c r="B122" s="49"/>
+      <c r="B122" s="2"/>
       <c r="C122" s="13"/>
       <c r="D122" s="2"/>
       <c r="E122" s="6"/>
-      <c r="F122" s="49"/>
-      <c r="G122" s="31"/>
+      <c r="F122" s="2"/>
+      <c r="G122" s="29"/>
       <c r="H122" s="2"/>
     </row>
     <row r="123" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A123" s="6"/>
-      <c r="B123" s="49"/>
+      <c r="B123" s="2"/>
       <c r="C123" s="13"/>
       <c r="D123" s="2"/>
       <c r="E123" s="6"/>
-      <c r="F123" s="49"/>
-      <c r="G123" s="31"/>
+      <c r="F123" s="2"/>
+      <c r="G123" s="29"/>
       <c r="H123" s="2"/>
     </row>
     <row r="124" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A124" s="6"/>
-      <c r="B124" s="49"/>
+      <c r="B124" s="2"/>
       <c r="C124" s="13"/>
       <c r="D124" s="2"/>
       <c r="E124" s="6"/>
-      <c r="F124" s="49"/>
-      <c r="G124" s="31"/>
+      <c r="F124" s="2"/>
+      <c r="G124" s="29"/>
       <c r="H124" s="2"/>
     </row>
     <row r="125" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A125" s="6"/>
-      <c r="B125" s="49"/>
-      <c r="C125" s="41"/>
+      <c r="B125" s="2"/>
+      <c r="C125" s="39"/>
       <c r="D125" s="2"/>
       <c r="E125" s="6"/>
-      <c r="F125" s="49"/>
-      <c r="G125" s="31"/>
+      <c r="F125" s="2"/>
+      <c r="G125" s="29"/>
       <c r="H125" s="2"/>
     </row>
     <row r="126" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A126" s="6"/>
-      <c r="B126" s="49"/>
-      <c r="C126" s="41"/>
+      <c r="B126" s="2"/>
+      <c r="C126" s="39"/>
       <c r="D126" s="2"/>
       <c r="E126" s="6"/>
-      <c r="F126" s="49"/>
-      <c r="G126" s="31"/>
+      <c r="F126" s="2"/>
+      <c r="G126" s="29"/>
       <c r="H126" s="2"/>
     </row>
     <row r="127" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A127" s="6"/>
-      <c r="B127" s="49"/>
-      <c r="C127" s="41"/>
+      <c r="B127" s="2"/>
+      <c r="C127" s="39"/>
       <c r="D127" s="2"/>
       <c r="E127" s="6"/>
-      <c r="F127" s="49"/>
-      <c r="G127" s="31"/>
+      <c r="F127" s="2"/>
+      <c r="G127" s="29"/>
       <c r="H127" s="2"/>
     </row>
     <row r="128" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A128" s="6"/>
-      <c r="B128" s="49"/>
-      <c r="C128" s="41"/>
+      <c r="B128" s="2"/>
+      <c r="C128" s="39"/>
       <c r="D128" s="2"/>
       <c r="E128" s="6"/>
-      <c r="F128" s="49"/>
-      <c r="G128" s="32"/>
+      <c r="F128" s="2"/>
+      <c r="G128" s="30"/>
       <c r="H128" s="2"/>
     </row>
     <row r="129" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A129" s="6"/>
-      <c r="B129" s="49"/>
-      <c r="C129" s="41"/>
+      <c r="B129" s="2"/>
+      <c r="C129" s="39"/>
       <c r="D129" s="2"/>
       <c r="E129" s="6"/>
-      <c r="F129" s="49"/>
-      <c r="G129" s="32"/>
+      <c r="F129" s="2"/>
+      <c r="G129" s="30"/>
       <c r="H129" s="2"/>
     </row>
     <row r="130" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A130" s="6"/>
-      <c r="B130" s="49"/>
-      <c r="C130" s="41"/>
+      <c r="B130" s="2"/>
+      <c r="C130" s="39"/>
       <c r="D130" s="2"/>
       <c r="E130" s="6"/>
-      <c r="F130" s="49"/>
-      <c r="G130" s="32"/>
+      <c r="F130" s="2"/>
+      <c r="G130" s="30"/>
       <c r="H130" s="2"/>
     </row>
     <row r="131" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A131" s="6"/>
-      <c r="B131" s="49"/>
-      <c r="C131" s="41"/>
+      <c r="B131" s="2"/>
+      <c r="C131" s="39"/>
       <c r="D131" s="2"/>
       <c r="E131" s="6"/>
-      <c r="F131" s="49"/>
-      <c r="G131" s="32"/>
+      <c r="F131" s="2"/>
+      <c r="G131" s="30"/>
       <c r="H131" s="2"/>
     </row>
     <row r="132" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A132" s="6"/>
-      <c r="B132" s="49"/>
-      <c r="C132" s="42"/>
+      <c r="B132" s="2"/>
+      <c r="C132" s="40"/>
       <c r="D132" s="2"/>
       <c r="E132" s="6"/>
-      <c r="F132" s="49"/>
-      <c r="G132" s="32"/>
+      <c r="F132" s="2"/>
+      <c r="G132" s="30"/>
       <c r="H132" s="2"/>
     </row>
     <row r="133" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A133" s="6"/>
-      <c r="B133" s="49"/>
-      <c r="C133" s="42"/>
+      <c r="B133" s="2"/>
+      <c r="C133" s="40"/>
       <c r="D133" s="2"/>
       <c r="E133" s="6"/>
-      <c r="F133" s="49"/>
-      <c r="G133" s="32"/>
+      <c r="F133" s="2"/>
+      <c r="G133" s="30"/>
       <c r="H133" s="2"/>
     </row>
     <row r="134" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A134" s="6"/>
-      <c r="B134" s="49"/>
-      <c r="C134" s="42"/>
+      <c r="B134" s="2"/>
+      <c r="C134" s="40"/>
       <c r="D134" s="2"/>
       <c r="E134" s="6"/>
-      <c r="F134" s="49"/>
-      <c r="G134" s="32"/>
+      <c r="F134" s="2"/>
+      <c r="G134" s="30"/>
       <c r="H134" s="2"/>
     </row>
     <row r="135" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A135" s="6"/>
-      <c r="B135" s="49"/>
-      <c r="C135" s="42"/>
+      <c r="B135" s="2"/>
+      <c r="C135" s="40"/>
       <c r="D135" s="2"/>
       <c r="E135" s="6"/>
-      <c r="F135" s="49"/>
-      <c r="G135" s="33"/>
+      <c r="F135" s="2"/>
+      <c r="G135" s="31"/>
       <c r="H135" s="2"/>
     </row>
     <row r="136" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A136" s="6"/>
-      <c r="B136" s="49"/>
-      <c r="C136" s="42"/>
+      <c r="B136" s="2"/>
+      <c r="C136" s="40"/>
       <c r="D136" s="2"/>
       <c r="E136" s="6"/>
-      <c r="F136" s="49"/>
-      <c r="G136" s="33"/>
+      <c r="F136" s="2"/>
+      <c r="G136" s="31"/>
       <c r="H136" s="2"/>
     </row>
     <row r="137" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A137" s="6"/>
-      <c r="B137" s="49"/>
-      <c r="C137" s="42"/>
+      <c r="B137" s="2"/>
+      <c r="C137" s="40"/>
       <c r="D137" s="2"/>
       <c r="E137" s="6"/>
-      <c r="F137" s="49"/>
-      <c r="G137" s="33"/>
+      <c r="F137" s="2"/>
+      <c r="G137" s="31"/>
       <c r="H137" s="2"/>
     </row>
     <row r="138" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A138" s="6"/>
-      <c r="B138" s="49"/>
-      <c r="C138" s="42"/>
+      <c r="B138" s="2"/>
+      <c r="C138" s="40"/>
       <c r="D138" s="2"/>
       <c r="E138" s="6"/>
-      <c r="F138" s="49"/>
-      <c r="G138" s="33"/>
+      <c r="F138" s="2"/>
+      <c r="G138" s="31"/>
       <c r="H138" s="2"/>
     </row>
     <row r="139" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A139" s="6"/>
-      <c r="B139" s="49"/>
-      <c r="C139" s="42"/>
+      <c r="B139" s="2"/>
+      <c r="C139" s="40"/>
       <c r="D139" s="2"/>
       <c r="E139" s="6"/>
-      <c r="F139" s="49"/>
-      <c r="G139" s="33"/>
+      <c r="F139" s="2"/>
+      <c r="G139" s="31"/>
       <c r="H139" s="2"/>
     </row>
     <row r="140" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A140" s="6"/>
-      <c r="B140" s="49"/>
-      <c r="C140" s="43"/>
+      <c r="B140" s="2"/>
+      <c r="C140" s="41"/>
       <c r="D140" s="2"/>
       <c r="E140" s="6"/>
-      <c r="F140" s="49"/>
-      <c r="G140" s="33"/>
+      <c r="F140" s="2"/>
+      <c r="G140" s="31"/>
       <c r="H140" s="2"/>
     </row>
     <row r="141" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A141" s="6"/>
-      <c r="B141" s="49"/>
-      <c r="C141" s="43"/>
+      <c r="B141" s="2"/>
+      <c r="C141" s="41"/>
       <c r="D141" s="2"/>
       <c r="E141" s="6"/>
-      <c r="F141" s="49"/>
-      <c r="G141" s="33"/>
+      <c r="F141" s="2"/>
+      <c r="G141" s="31"/>
       <c r="H141" s="2"/>
     </row>
     <row r="142" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A142" s="6"/>
-      <c r="B142" s="49"/>
-      <c r="C142" s="43"/>
+      <c r="B142" s="2"/>
+      <c r="C142" s="41"/>
       <c r="D142" s="2"/>
       <c r="E142" s="6"/>
-      <c r="F142" s="49"/>
-      <c r="G142" s="33"/>
+      <c r="F142" s="2"/>
+      <c r="G142" s="31"/>
       <c r="H142" s="2"/>
     </row>
     <row r="143" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A143" s="6"/>
-      <c r="B143" s="49"/>
-      <c r="C143" s="43"/>
+      <c r="B143" s="2"/>
+      <c r="C143" s="41"/>
       <c r="D143" s="2"/>
       <c r="E143" s="6"/>
-      <c r="F143" s="49"/>
+      <c r="F143" s="2"/>
       <c r="G143" s="16"/>
       <c r="H143" s="2"/>
     </row>
     <row r="144" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A144" s="6"/>
-      <c r="B144" s="49"/>
-      <c r="C144" s="44"/>
+      <c r="B144" s="2"/>
+      <c r="C144" s="42"/>
       <c r="D144" s="2"/>
       <c r="E144" s="6"/>
-      <c r="F144" s="49"/>
+      <c r="F144" s="2"/>
       <c r="G144" s="16"/>
       <c r="H144" s="2"/>
     </row>
     <row r="145" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A145" s="6"/>
-      <c r="B145" s="49"/>
-      <c r="C145" s="44"/>
+      <c r="B145" s="2"/>
+      <c r="C145" s="42"/>
       <c r="D145" s="2"/>
       <c r="E145" s="6"/>
-      <c r="F145" s="49"/>
+      <c r="F145" s="2"/>
       <c r="G145" s="16"/>
       <c r="H145" s="2"/>
     </row>
     <row r="146" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A146" s="6"/>
-      <c r="B146" s="49"/>
-      <c r="C146" s="44"/>
+      <c r="B146" s="2"/>
+      <c r="C146" s="42"/>
       <c r="D146" s="2"/>
       <c r="E146" s="6"/>
-      <c r="F146" s="49"/>
+      <c r="F146" s="2"/>
       <c r="G146" s="17"/>
       <c r="H146" s="2"/>
     </row>
     <row r="147" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A147" s="6"/>
-      <c r="B147" s="49"/>
-      <c r="C147" s="44"/>
+      <c r="B147" s="2"/>
+      <c r="C147" s="42"/>
       <c r="D147" s="2"/>
       <c r="E147" s="6"/>
-      <c r="F147" s="49"/>
+      <c r="F147" s="2"/>
       <c r="G147" s="17"/>
       <c r="H147" s="2"/>
     </row>
     <row r="148" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A148" s="6"/>
-      <c r="B148" s="49"/>
-      <c r="C148" s="45"/>
+      <c r="B148" s="2"/>
+      <c r="C148" s="43"/>
       <c r="D148" s="2"/>
       <c r="E148" s="6"/>
-      <c r="F148" s="49"/>
+      <c r="F148" s="2"/>
       <c r="G148" s="17"/>
       <c r="H148" s="2"/>
     </row>
     <row r="149" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A149" s="6"/>
-      <c r="B149" s="49"/>
-      <c r="C149" s="45"/>
+      <c r="B149" s="2"/>
+      <c r="C149" s="43"/>
       <c r="D149" s="2"/>
       <c r="E149" s="6"/>
-      <c r="F149" s="49"/>
+      <c r="F149" s="2"/>
       <c r="G149" s="17"/>
       <c r="H149" s="2"/>
     </row>
     <row r="150" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A150" s="6"/>
-      <c r="B150" s="49"/>
-      <c r="C150" s="46"/>
+      <c r="B150" s="2"/>
+      <c r="C150" s="44"/>
       <c r="D150" s="2"/>
       <c r="E150" s="6"/>
-      <c r="F150" s="49"/>
-      <c r="G150" s="34"/>
+      <c r="F150" s="2"/>
+      <c r="G150" s="32"/>
       <c r="H150" s="8"/>
     </row>
     <row r="151" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A151" s="6"/>
-      <c r="B151" s="49"/>
-      <c r="C151" s="46"/>
+      <c r="B151" s="2"/>
+      <c r="C151" s="44"/>
       <c r="D151" s="8"/>
       <c r="E151" s="6"/>
-      <c r="F151" s="49"/>
-      <c r="G151" s="34"/>
+      <c r="F151" s="2"/>
+      <c r="G151" s="32"/>
       <c r="H151" s="13"/>
     </row>
     <row r="152" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A152" s="10"/>
-      <c r="B152" s="50"/>
+      <c r="B152" s="13"/>
       <c r="C152" s="7"/>
       <c r="D152" s="13"/>
       <c r="E152" s="6"/>
-      <c r="F152" s="49"/>
-      <c r="G152" s="34"/>
+      <c r="F152" s="2"/>
+      <c r="G152" s="32"/>
       <c r="H152" s="2"/>
     </row>
     <row r="153" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A153" s="6"/>
-      <c r="B153" s="49"/>
+      <c r="B153" s="2"/>
       <c r="C153" s="7"/>
       <c r="D153" s="2"/>
       <c r="E153" s="6"/>
-      <c r="F153" s="49"/>
-      <c r="G153" s="34"/>
+      <c r="F153" s="2"/>
+      <c r="G153" s="32"/>
       <c r="H153" s="2"/>
     </row>
     <row r="154" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A154" s="6"/>
-      <c r="B154" s="49"/>
+      <c r="B154" s="2"/>
       <c r="C154" s="7"/>
       <c r="D154" s="2"/>
       <c r="E154" s="6"/>
-      <c r="F154" s="49"/>
-      <c r="G154" s="34"/>
+      <c r="F154" s="2"/>
+      <c r="G154" s="32"/>
       <c r="H154" s="2"/>
     </row>
     <row r="155" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A155" s="6"/>
-      <c r="B155" s="49"/>
+      <c r="B155" s="2"/>
       <c r="C155" s="7"/>
       <c r="D155" s="2"/>
       <c r="E155" s="6"/>
-      <c r="F155" s="49"/>
-      <c r="G155" s="34"/>
+      <c r="F155" s="2"/>
+      <c r="G155" s="32"/>
       <c r="H155" s="2"/>
     </row>
     <row r="156" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A156" s="6"/>
-      <c r="B156" s="49"/>
+      <c r="B156" s="2"/>
       <c r="C156" s="7"/>
       <c r="D156" s="2"/>
       <c r="E156" s="6"/>
-      <c r="F156" s="49"/>
-      <c r="G156" s="35"/>
+      <c r="F156" s="2"/>
+      <c r="G156" s="33"/>
       <c r="H156" s="2"/>
     </row>
     <row r="157" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A157" s="6"/>
-      <c r="B157" s="49"/>
+      <c r="B157" s="2"/>
       <c r="C157" s="7"/>
       <c r="D157" s="2"/>
       <c r="E157" s="6"/>
-      <c r="F157" s="49"/>
-      <c r="G157" s="35"/>
+      <c r="F157" s="2"/>
+      <c r="G157" s="33"/>
       <c r="H157" s="2"/>
     </row>
     <row r="158" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A158" s="6"/>
-      <c r="B158" s="49"/>
+      <c r="B158" s="2"/>
       <c r="C158" s="7"/>
       <c r="D158" s="2"/>
       <c r="E158" s="6"/>
-      <c r="F158" s="49"/>
-      <c r="G158" s="35"/>
+      <c r="F158" s="2"/>
+      <c r="G158" s="33"/>
       <c r="H158" s="2"/>
     </row>
     <row r="159" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A159" s="6"/>
-      <c r="B159" s="49"/>
+      <c r="B159" s="2"/>
       <c r="C159" s="7"/>
       <c r="D159" s="2"/>
       <c r="E159" s="6"/>
-      <c r="F159" s="49"/>
-      <c r="G159" s="35"/>
+      <c r="F159" s="2"/>
+      <c r="G159" s="33"/>
       <c r="H159" s="2"/>
     </row>
     <row r="160" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A160" s="6"/>
-      <c r="B160" s="49"/>
-      <c r="C160" s="47"/>
+      <c r="B160" s="2"/>
+      <c r="C160" s="45"/>
       <c r="D160" s="2"/>
       <c r="E160" s="6"/>
-      <c r="F160" s="49"/>
-      <c r="G160" s="35"/>
+      <c r="F160" s="2"/>
+      <c r="G160" s="33"/>
       <c r="H160" s="2"/>
     </row>
     <row r="161" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A161" s="6"/>
-      <c r="B161" s="49"/>
+      <c r="B161" s="2"/>
       <c r="D161" s="2"/>
       <c r="E161" s="6"/>
-      <c r="F161" s="49"/>
-      <c r="G161" s="35"/>
+      <c r="F161" s="2"/>
+      <c r="G161" s="33"/>
       <c r="H161" s="2"/>
     </row>
     <row r="162" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A162" s="6"/>
-      <c r="B162" s="49"/>
+      <c r="B162" s="2"/>
       <c r="D162" s="2"/>
       <c r="E162" s="6"/>
-      <c r="F162" s="49"/>
-      <c r="G162" s="35"/>
+      <c r="F162" s="2"/>
+      <c r="G162" s="33"/>
       <c r="H162" s="2"/>
     </row>
     <row r="163" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A163" s="6"/>
-      <c r="B163" s="49"/>
+      <c r="B163" s="2"/>
       <c r="D163" s="2"/>
       <c r="E163" s="6"/>
-      <c r="F163" s="49"/>
-      <c r="G163" s="35"/>
+      <c r="F163" s="2"/>
+      <c r="G163" s="33"/>
       <c r="H163" s="2"/>
     </row>
     <row r="164" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A164" s="6"/>
-      <c r="B164" s="49"/>
+      <c r="B164" s="2"/>
       <c r="D164" s="2"/>
       <c r="E164" s="6"/>
-      <c r="F164" s="49"/>
-      <c r="G164" s="35"/>
+      <c r="F164" s="2"/>
+      <c r="G164" s="33"/>
       <c r="H164" s="2"/>
     </row>
     <row r="165" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A165" s="6"/>
-      <c r="B165" s="49"/>
+      <c r="B165" s="2"/>
       <c r="D165" s="2"/>
       <c r="E165" s="6"/>
-      <c r="F165" s="49"/>
-      <c r="G165" s="35"/>
+      <c r="F165" s="2"/>
+      <c r="G165" s="33"/>
       <c r="H165" s="2"/>
     </row>
     <row r="166" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A166" s="6"/>
-      <c r="B166" s="49"/>
+      <c r="B166" s="2"/>
       <c r="D166" s="2"/>
       <c r="E166" s="6"/>
-      <c r="F166" s="49"/>
-      <c r="G166" s="35"/>
+      <c r="F166" s="2"/>
+      <c r="G166" s="33"/>
       <c r="H166" s="2"/>
     </row>
     <row r="167" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A167" s="6"/>
-      <c r="B167" s="49"/>
+      <c r="B167" s="2"/>
       <c r="D167" s="2"/>
       <c r="E167" s="6"/>
-      <c r="F167" s="49"/>
-      <c r="G167" s="36"/>
+      <c r="F167" s="2"/>
+      <c r="G167" s="34"/>
       <c r="H167" s="2"/>
     </row>
     <row r="168" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A168" s="6"/>
-      <c r="B168" s="49"/>
+      <c r="B168" s="2"/>
       <c r="D168" s="2"/>
       <c r="E168" s="6"/>
-      <c r="F168" s="49"/>
-      <c r="G168" s="36"/>
+      <c r="F168" s="2"/>
+      <c r="G168" s="34"/>
       <c r="H168" s="2"/>
     </row>
     <row r="169" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A169" s="6"/>
-      <c r="B169" s="49"/>
+      <c r="B169" s="2"/>
       <c r="D169" s="2"/>
       <c r="E169" s="6"/>
-      <c r="F169" s="49"/>
-      <c r="G169" s="37"/>
+      <c r="F169" s="2"/>
+      <c r="G169" s="35"/>
       <c r="H169" s="2"/>
     </row>
     <row r="170" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A170" s="6"/>
-      <c r="B170" s="49"/>
+      <c r="B170" s="2"/>
       <c r="D170" s="2"/>
       <c r="E170" s="6"/>
-      <c r="F170" s="49"/>
-      <c r="G170" s="37"/>
+      <c r="F170" s="2"/>
+      <c r="G170" s="35"/>
       <c r="H170" s="2"/>
     </row>
     <row r="171" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A171" s="6"/>
-      <c r="B171" s="49"/>
+      <c r="B171" s="2"/>
       <c r="D171" s="2"/>
       <c r="E171" s="6"/>
-      <c r="F171" s="49"/>
-      <c r="G171" s="37"/>
+      <c r="F171" s="2"/>
+      <c r="G171" s="35"/>
       <c r="H171" s="2"/>
     </row>
     <row r="172" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A172" s="6"/>
-      <c r="B172" s="49"/>
+      <c r="B172" s="2"/>
       <c r="D172" s="2"/>
       <c r="E172" s="6"/>
-      <c r="F172" s="49"/>
-      <c r="G172" s="37"/>
+      <c r="F172" s="2"/>
+      <c r="G172" s="35"/>
       <c r="H172" s="2"/>
     </row>
     <row r="173" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A173" s="6"/>
-      <c r="B173" s="49"/>
+      <c r="B173" s="2"/>
       <c r="D173" s="2"/>
       <c r="E173" s="6"/>
-      <c r="F173" s="49"/>
-      <c r="G173" s="37"/>
+      <c r="F173" s="2"/>
+      <c r="G173" s="35"/>
       <c r="H173" s="2"/>
     </row>
     <row r="174" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A174" s="6"/>
-      <c r="B174" s="49"/>
+      <c r="B174" s="2"/>
       <c r="D174" s="2"/>
       <c r="E174" s="6"/>
-      <c r="F174" s="49"/>
-      <c r="G174" s="37"/>
+      <c r="F174" s="2"/>
+      <c r="G174" s="35"/>
       <c r="H174" s="2"/>
     </row>
     <row r="175" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A175" s="6"/>
-      <c r="B175" s="49"/>
+      <c r="B175" s="2"/>
       <c r="D175" s="2"/>
       <c r="E175" s="6"/>
-      <c r="F175" s="49"/>
-      <c r="G175" s="38"/>
+      <c r="F175" s="2"/>
+      <c r="G175" s="36"/>
       <c r="H175" s="2"/>
     </row>
     <row r="176" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A176" s="6"/>
-      <c r="B176" s="49"/>
+      <c r="B176" s="2"/>
       <c r="D176" s="2"/>
       <c r="E176" s="6"/>
-      <c r="F176" s="49"/>
-      <c r="G176" s="38"/>
+      <c r="F176" s="2"/>
+      <c r="G176" s="36"/>
       <c r="H176" s="2"/>
     </row>
     <row r="177" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A177" s="6"/>
-      <c r="B177" s="49"/>
+      <c r="B177" s="2"/>
       <c r="D177" s="2"/>
       <c r="E177" s="6"/>
-      <c r="F177" s="49"/>
-      <c r="G177" s="38"/>
+      <c r="F177" s="2"/>
+      <c r="G177" s="36"/>
       <c r="H177" s="2"/>
     </row>
     <row r="178" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A178" s="6"/>
-      <c r="B178" s="49"/>
+      <c r="B178" s="2"/>
       <c r="D178" s="2"/>
       <c r="E178" s="6"/>
-      <c r="F178" s="49"/>
-      <c r="G178" s="38"/>
+      <c r="F178" s="2"/>
+      <c r="G178" s="36"/>
       <c r="H178" s="2"/>
     </row>
     <row r="179" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A179" s="6"/>
-      <c r="B179" s="49"/>
+      <c r="B179" s="2"/>
       <c r="D179" s="2"/>
       <c r="E179" s="6"/>
-      <c r="F179" s="49"/>
-      <c r="G179" s="38"/>
+      <c r="F179" s="2"/>
+      <c r="G179" s="36"/>
       <c r="H179" s="2"/>
     </row>
     <row r="180" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A180" s="6"/>
-      <c r="B180" s="49"/>
+      <c r="B180" s="2"/>
       <c r="D180" s="2"/>
       <c r="E180" s="6"/>
-      <c r="F180" s="49"/>
-      <c r="G180" s="37"/>
+      <c r="F180" s="2"/>
+      <c r="G180" s="35"/>
       <c r="H180" s="2"/>
     </row>
     <row r="181" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A181" s="6"/>
-      <c r="B181" s="49"/>
+      <c r="B181" s="2"/>
       <c r="D181" s="2"/>
       <c r="E181" s="6"/>
-      <c r="F181" s="49"/>
-      <c r="G181" s="37"/>
+      <c r="F181" s="2"/>
+      <c r="G181" s="35"/>
       <c r="H181" s="2"/>
     </row>
     <row r="182" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A182" s="6"/>
-      <c r="B182" s="49"/>
+      <c r="B182" s="2"/>
       <c r="D182" s="2"/>
       <c r="E182" s="6"/>
-      <c r="F182" s="49"/>
-      <c r="G182" s="37"/>
+      <c r="F182" s="2"/>
+      <c r="G182" s="35"/>
       <c r="H182" s="2"/>
     </row>
     <row r="183" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A183" s="6"/>
-      <c r="B183" s="49"/>
+      <c r="B183" s="2"/>
       <c r="D183" s="2"/>
       <c r="E183" s="6"/>
-      <c r="F183" s="49"/>
-      <c r="G183" s="37"/>
+      <c r="F183" s="2"/>
+      <c r="G183" s="35"/>
       <c r="H183" s="2"/>
     </row>
     <row r="184" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A184" s="6"/>
-      <c r="B184" s="49"/>
+      <c r="B184" s="2"/>
       <c r="D184" s="2"/>
       <c r="E184" s="6"/>
-      <c r="F184" s="49"/>
-      <c r="G184" s="38"/>
+      <c r="F184" s="2"/>
+      <c r="G184" s="36"/>
       <c r="H184" s="2"/>
     </row>
     <row r="185" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A185" s="6"/>
-      <c r="B185" s="49"/>
+      <c r="B185" s="2"/>
       <c r="D185" s="2"/>
       <c r="E185" s="6"/>
-      <c r="F185" s="49"/>
-      <c r="G185" s="39"/>
+      <c r="F185" s="2"/>
+      <c r="G185" s="37"/>
       <c r="H185" s="2"/>
     </row>
     <row r="186" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A186" s="6"/>
-      <c r="B186" s="49"/>
+      <c r="B186" s="2"/>
       <c r="D186" s="2"/>
       <c r="E186" s="6"/>
-      <c r="F186" s="49"/>
-      <c r="G186" s="40"/>
+      <c r="F186" s="2"/>
+      <c r="G186" s="38"/>
       <c r="H186" s="2"/>
     </row>
     <row r="187" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A187" s="6"/>
-      <c r="B187" s="49"/>
+      <c r="B187" s="2"/>
       <c r="D187" s="2"/>
       <c r="E187" s="6"/>
-      <c r="F187" s="49"/>
-      <c r="G187" s="40"/>
+      <c r="F187" s="2"/>
+      <c r="G187" s="38"/>
       <c r="H187" s="2"/>
     </row>
     <row r="188" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A188" s="6"/>
-      <c r="B188" s="49"/>
+      <c r="B188" s="2"/>
       <c r="D188" s="2"/>
       <c r="E188" s="6"/>
-      <c r="F188" s="49"/>
-      <c r="G188" s="40"/>
+      <c r="F188" s="2"/>
+      <c r="G188" s="38"/>
       <c r="H188" s="2"/>
     </row>
     <row r="189" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A189" s="6"/>
-      <c r="B189" s="49"/>
+      <c r="B189" s="2"/>
       <c r="D189" s="2"/>
       <c r="E189" s="6"/>
-      <c r="F189" s="49"/>
-      <c r="G189" s="40"/>
+      <c r="F189" s="2"/>
+      <c r="G189" s="38"/>
       <c r="H189" s="2"/>
     </row>
     <row r="190" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A190" s="6"/>
-      <c r="B190" s="49"/>
+      <c r="B190" s="2"/>
       <c r="D190" s="2"/>
       <c r="E190" s="6"/>
-      <c r="F190" s="49"/>
-      <c r="G190" s="40"/>
+      <c r="F190" s="2"/>
+      <c r="G190" s="38"/>
       <c r="H190" s="2"/>
     </row>
     <row r="191" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A191" s="6"/>
-      <c r="B191" s="49"/>
+      <c r="B191" s="2"/>
       <c r="D191" s="2"/>
       <c r="E191" s="6"/>
-      <c r="F191" s="49"/>
-      <c r="G191" s="40"/>
+      <c r="F191" s="2"/>
+      <c r="G191" s="38"/>
       <c r="H191" s="2"/>
     </row>
     <row r="192" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A192" s="6"/>
-      <c r="B192" s="49"/>
+      <c r="B192" s="2"/>
       <c r="D192" s="2"/>
       <c r="E192" s="6"/>
-      <c r="F192" s="49"/>
-      <c r="G192" s="40"/>
+      <c r="F192" s="2"/>
+      <c r="G192" s="38"/>
       <c r="H192" s="2"/>
     </row>
     <row r="193" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A193" s="6"/>
-      <c r="B193" s="49"/>
+      <c r="B193" s="2"/>
       <c r="D193" s="2"/>
       <c r="E193" s="6"/>
-      <c r="F193" s="49"/>
-      <c r="G193" s="40"/>
+      <c r="F193" s="2"/>
+      <c r="G193" s="38"/>
       <c r="H193" s="2"/>
     </row>
     <row r="194" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A194" s="6"/>
-      <c r="B194" s="49"/>
+      <c r="B194" s="2"/>
       <c r="D194" s="2"/>
       <c r="E194" s="6"/>
-      <c r="F194" s="49"/>
-      <c r="G194" s="40"/>
+      <c r="F194" s="2"/>
+      <c r="G194" s="38"/>
       <c r="H194" s="2"/>
     </row>
     <row r="195" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A195" s="6"/>
-      <c r="B195" s="49"/>
+      <c r="B195" s="2"/>
       <c r="D195" s="2"/>
       <c r="E195" s="6"/>
-      <c r="F195" s="49"/>
-      <c r="G195" s="40"/>
+      <c r="F195" s="2"/>
+      <c r="G195" s="38"/>
       <c r="H195" s="2"/>
     </row>
     <row r="196" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A196" s="6"/>
-      <c r="B196" s="49"/>
+      <c r="B196" s="2"/>
       <c r="D196" s="2"/>
       <c r="E196" s="6"/>
-      <c r="F196" s="49"/>
-      <c r="G196" s="40"/>
+      <c r="F196" s="2"/>
+      <c r="G196" s="38"/>
       <c r="H196" s="2"/>
     </row>
     <row r="197" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A197" s="6"/>
-      <c r="B197" s="49"/>
+      <c r="B197" s="2"/>
       <c r="D197" s="2"/>
       <c r="E197" s="6"/>
-      <c r="F197" s="49"/>
-      <c r="G197" s="40"/>
+      <c r="F197" s="2"/>
+      <c r="G197" s="38"/>
       <c r="H197" s="2"/>
     </row>
     <row r="198" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A198" s="6"/>
-      <c r="B198" s="49"/>
+      <c r="B198" s="2"/>
       <c r="D198" s="2"/>
       <c r="E198" s="6"/>
-      <c r="F198" s="49"/>
+      <c r="F198" s="2"/>
       <c r="G198" s="18"/>
       <c r="H198" s="2"/>
     </row>
     <row r="199" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A199" s="6"/>
-      <c r="B199" s="49"/>
+      <c r="B199" s="2"/>
       <c r="D199" s="2"/>
       <c r="E199" s="6"/>
-      <c r="F199" s="49"/>
+      <c r="F199" s="2"/>
       <c r="G199" s="18"/>
       <c r="H199" s="2"/>
     </row>
     <row r="200" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A200" s="6"/>
-      <c r="B200" s="49"/>
+      <c r="B200" s="2"/>
       <c r="D200" s="2"/>
       <c r="E200" s="6"/>
-      <c r="F200" s="49"/>
+      <c r="F200" s="2"/>
       <c r="G200" s="18"/>
       <c r="H200" s="2"/>
     </row>
     <row r="201" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A201" s="6"/>
-      <c r="B201" s="49"/>
+      <c r="B201" s="2"/>
       <c r="D201" s="2"/>
       <c r="E201" s="6"/>
-      <c r="F201" s="49"/>
+      <c r="F201" s="2"/>
       <c r="G201" s="18"/>
       <c r="H201" s="13"/>
     </row>
     <row r="202" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="12"/>
-      <c r="B202" s="50"/>
+      <c r="B202" s="13"/>
       <c r="D202" s="13"/>
       <c r="E202" s="6"/>
-      <c r="F202" s="49"/>
+      <c r="F202" s="2"/>
       <c r="G202" s="18"/>
       <c r="H202" s="3"/>
     </row>
     <row r="203" spans="1:8" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D203" s="3"/>
       <c r="E203" s="6"/>
-      <c r="F203" s="49"/>
+      <c r="F203" s="2"/>
       <c r="G203" s="13"/>
       <c r="H203" s="2"/>
     </row>
     <row r="204" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D204" s="2"/>
       <c r="E204" s="6"/>
-      <c r="F204" s="49"/>
+      <c r="F204" s="2"/>
       <c r="G204" s="13"/>
       <c r="H204" s="2"/>
     </row>
     <row r="205" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D205" s="2"/>
       <c r="E205" s="6"/>
-      <c r="F205" s="49"/>
+      <c r="F205" s="2"/>
       <c r="G205" s="13"/>
       <c r="H205" s="2"/>
     </row>
     <row r="206" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D206" s="2"/>
       <c r="E206" s="6"/>
-      <c r="F206" s="49"/>
+      <c r="F206" s="2"/>
       <c r="G206" s="13"/>
       <c r="H206" s="2"/>
     </row>
     <row r="207" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D207" s="2"/>
       <c r="E207" s="6"/>
-      <c r="F207" s="49"/>
+      <c r="F207" s="2"/>
       <c r="G207" s="13"/>
       <c r="H207" s="2"/>
     </row>
     <row r="208" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D208" s="2"/>
       <c r="E208" s="6"/>
-      <c r="F208" s="49"/>
-      <c r="G208" s="41"/>
+      <c r="F208" s="2"/>
+      <c r="G208" s="39"/>
       <c r="H208" s="2"/>
     </row>
     <row r="209" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D209" s="2"/>
       <c r="E209" s="6"/>
-      <c r="F209" s="49"/>
-      <c r="G209" s="41"/>
+      <c r="F209" s="2"/>
+      <c r="G209" s="39"/>
       <c r="H209" s="2"/>
     </row>
     <row r="210" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D210" s="2"/>
       <c r="E210" s="6"/>
-      <c r="F210" s="49"/>
-      <c r="G210" s="41"/>
+      <c r="F210" s="2"/>
+      <c r="G210" s="39"/>
       <c r="H210" s="2"/>
     </row>
     <row r="211" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D211" s="2"/>
       <c r="E211" s="6"/>
-      <c r="F211" s="49"/>
-      <c r="G211" s="41"/>
+      <c r="F211" s="2"/>
+      <c r="G211" s="39"/>
       <c r="H211" s="2"/>
     </row>
     <row r="212" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D212" s="2"/>
       <c r="E212" s="6"/>
-      <c r="F212" s="49"/>
-      <c r="G212" s="41"/>
+      <c r="F212" s="2"/>
+      <c r="G212" s="39"/>
       <c r="H212" s="2"/>
     </row>
     <row r="213" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D213" s="2"/>
       <c r="E213" s="6"/>
-      <c r="F213" s="49"/>
-      <c r="G213" s="41"/>
+      <c r="F213" s="2"/>
+      <c r="G213" s="39"/>
       <c r="H213" s="2"/>
     </row>
     <row r="214" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D214" s="2"/>
       <c r="E214" s="6"/>
-      <c r="F214" s="49"/>
-      <c r="G214" s="41"/>
+      <c r="F214" s="2"/>
+      <c r="G214" s="39"/>
       <c r="H214" s="2"/>
     </row>
     <row r="215" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D215" s="2"/>
       <c r="E215" s="6"/>
-      <c r="F215" s="49"/>
-      <c r="G215" s="42"/>
+      <c r="F215" s="2"/>
+      <c r="G215" s="40"/>
       <c r="H215" s="2"/>
     </row>
     <row r="216" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D216" s="2"/>
       <c r="E216" s="6"/>
-      <c r="F216" s="49"/>
-      <c r="G216" s="42"/>
+      <c r="F216" s="2"/>
+      <c r="G216" s="40"/>
       <c r="H216" s="2"/>
     </row>
     <row r="217" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D217" s="2"/>
       <c r="E217" s="6"/>
-      <c r="F217" s="49"/>
-      <c r="G217" s="42"/>
+      <c r="F217" s="2"/>
+      <c r="G217" s="40"/>
       <c r="H217" s="2"/>
     </row>
     <row r="218" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D218" s="2"/>
       <c r="E218" s="6"/>
-      <c r="F218" s="49"/>
-      <c r="G218" s="42"/>
+      <c r="F218" s="2"/>
+      <c r="G218" s="40"/>
       <c r="H218" s="2"/>
     </row>
     <row r="219" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D219" s="2"/>
       <c r="E219" s="6"/>
-      <c r="F219" s="49"/>
-      <c r="G219" s="42"/>
+      <c r="F219" s="2"/>
+      <c r="G219" s="40"/>
       <c r="H219" s="2"/>
     </row>
     <row r="220" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D220" s="2"/>
       <c r="E220" s="6"/>
-      <c r="F220" s="49"/>
-      <c r="G220" s="42"/>
+      <c r="F220" s="2"/>
+      <c r="G220" s="40"/>
       <c r="H220" s="2"/>
     </row>
     <row r="221" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D221" s="2"/>
       <c r="E221" s="6"/>
-      <c r="F221" s="49"/>
-      <c r="G221" s="42"/>
+      <c r="F221" s="2"/>
+      <c r="G221" s="40"/>
       <c r="H221" s="2"/>
     </row>
     <row r="222" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D222" s="2"/>
       <c r="E222" s="6"/>
-      <c r="F222" s="49"/>
-      <c r="G222" s="42"/>
+      <c r="F222" s="2"/>
+      <c r="G222" s="40"/>
       <c r="H222" s="2"/>
     </row>
     <row r="223" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D223" s="2"/>
       <c r="E223" s="6"/>
-      <c r="F223" s="49"/>
-      <c r="G223" s="42"/>
+      <c r="F223" s="2"/>
+      <c r="G223" s="40"/>
       <c r="H223" s="2"/>
     </row>
     <row r="224" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D224" s="2"/>
       <c r="E224" s="6"/>
-      <c r="F224" s="49"/>
-      <c r="G224" s="43"/>
+      <c r="F224" s="2"/>
+      <c r="G224" s="41"/>
       <c r="H224" s="2"/>
     </row>
     <row r="225" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D225" s="2"/>
       <c r="E225" s="6"/>
-      <c r="F225" s="49"/>
+      <c r="F225" s="2"/>
       <c r="G225" s="5"/>
       <c r="H225" s="2"/>
     </row>
     <row r="226" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D226" s="2"/>
       <c r="E226" s="6"/>
-      <c r="F226" s="49"/>
+      <c r="F226" s="2"/>
       <c r="G226" s="5"/>
       <c r="H226" s="2"/>
     </row>
     <row r="227" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D227" s="2"/>
       <c r="E227" s="6"/>
-      <c r="F227" s="49"/>
+      <c r="F227" s="2"/>
       <c r="G227" s="5"/>
       <c r="H227" s="2"/>
     </row>
     <row r="228" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D228" s="2"/>
       <c r="E228" s="6"/>
-      <c r="F228" s="49"/>
+      <c r="F228" s="2"/>
       <c r="G228" s="5"/>
       <c r="H228" s="2"/>
     </row>
     <row r="229" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D229" s="2"/>
       <c r="E229" s="6"/>
-      <c r="F229" s="49"/>
+      <c r="F229" s="2"/>
       <c r="G229" s="5"/>
       <c r="H229" s="2"/>
     </row>
     <row r="230" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D230" s="2"/>
       <c r="E230" s="6"/>
-      <c r="F230" s="49"/>
+      <c r="F230" s="2"/>
       <c r="G230" s="5"/>
       <c r="H230" s="2"/>
     </row>
     <row r="231" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D231" s="2"/>
       <c r="E231" s="6"/>
-      <c r="F231" s="49"/>
+      <c r="F231" s="2"/>
       <c r="G231" s="5"/>
       <c r="H231" s="2"/>
     </row>
     <row r="232" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D232" s="2"/>
       <c r="E232" s="6"/>
-      <c r="F232" s="49"/>
+      <c r="F232" s="2"/>
       <c r="G232" s="5"/>
       <c r="H232" s="2"/>
     </row>
     <row r="233" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D233" s="2"/>
       <c r="E233" s="6"/>
-      <c r="F233" s="49"/>
+      <c r="F233" s="2"/>
       <c r="G233" s="5"/>
       <c r="H233" s="2"/>
     </row>
     <row r="234" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D234" s="2"/>
       <c r="E234" s="6"/>
-      <c r="F234" s="49"/>
+      <c r="F234" s="2"/>
       <c r="H234" s="2"/>
     </row>
     <row r="235" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D235" s="2"/>
       <c r="E235" s="6"/>
-      <c r="F235" s="49"/>
+      <c r="F235" s="2"/>
       <c r="H235" s="2"/>
     </row>
     <row r="236" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D236" s="2"/>
       <c r="E236" s="6"/>
-      <c r="F236" s="49"/>
+      <c r="F236" s="2"/>
       <c r="H236" s="2"/>
     </row>
     <row r="237" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D237" s="2"/>
       <c r="E237" s="6"/>
-      <c r="F237" s="49"/>
+      <c r="F237" s="2"/>
       <c r="H237" s="2"/>
     </row>
     <row r="238" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D238" s="2"/>
       <c r="E238" s="6"/>
-      <c r="F238" s="49"/>
+      <c r="F238" s="2"/>
       <c r="H238" s="2"/>
     </row>
     <row r="239" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D239" s="2"/>
       <c r="E239" s="6"/>
-      <c r="F239" s="49"/>
+      <c r="F239" s="2"/>
       <c r="H239" s="2"/>
     </row>
     <row r="240" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D240" s="2"/>
       <c r="E240" s="6"/>
-      <c r="F240" s="49"/>
+      <c r="F240" s="2"/>
       <c r="H240" s="2"/>
     </row>
     <row r="241" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D241" s="2"/>
       <c r="E241" s="6"/>
-      <c r="F241" s="49"/>
+      <c r="F241" s="2"/>
       <c r="H241" s="2"/>
     </row>
     <row r="242" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D242" s="2"/>
       <c r="E242" s="6"/>
-      <c r="F242" s="49"/>
+      <c r="F242" s="2"/>
       <c r="H242" s="2"/>
     </row>
     <row r="243" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D243" s="2"/>
       <c r="E243" s="6"/>
-      <c r="F243" s="49"/>
+      <c r="F243" s="2"/>
       <c r="H243" s="2"/>
     </row>
     <row r="244" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D244" s="2"/>
       <c r="E244" s="6"/>
-      <c r="F244" s="49"/>
+      <c r="F244" s="2"/>
       <c r="H244" s="2"/>
     </row>
     <row r="245" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D245" s="2"/>
       <c r="E245" s="6"/>
-      <c r="F245" s="49"/>
+      <c r="F245" s="2"/>
       <c r="H245" s="2"/>
     </row>
     <row r="246" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D246" s="2"/>
       <c r="E246" s="6"/>
-      <c r="F246" s="49"/>
+      <c r="F246" s="2"/>
       <c r="H246" s="2"/>
     </row>
     <row r="247" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D247" s="2"/>
       <c r="E247" s="6"/>
-      <c r="F247" s="49"/>
+      <c r="F247" s="2"/>
       <c r="H247" s="2"/>
     </row>
     <row r="248" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D248" s="2"/>
       <c r="E248" s="6"/>
-      <c r="F248" s="49"/>
+      <c r="F248" s="2"/>
       <c r="H248" s="2"/>
     </row>
     <row r="249" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D249" s="2"/>
       <c r="E249" s="6"/>
-      <c r="F249" s="49"/>
+      <c r="F249" s="2"/>
       <c r="H249" s="2"/>
     </row>
     <row r="250" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D250" s="2"/>
       <c r="E250" s="6"/>
-      <c r="F250" s="49"/>
+      <c r="F250" s="2"/>
       <c r="H250" s="2"/>
     </row>
     <row r="251" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D251" s="2"/>
       <c r="E251" s="6"/>
-      <c r="F251" s="49"/>
+      <c r="F251" s="2"/>
       <c r="H251" s="13"/>
     </row>
     <row r="252" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D252" s="13"/>
       <c r="E252" s="6"/>
-      <c r="F252" s="49"/>
+      <c r="F252" s="2"/>
       <c r="H252" s="2"/>
     </row>
     <row r="253" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D253" s="2"/>
       <c r="E253" s="6"/>
-      <c r="F253" s="49"/>
+      <c r="F253" s="2"/>
       <c r="H253" s="2"/>
     </row>
     <row r="254" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D254" s="2"/>
       <c r="E254" s="6"/>
-      <c r="F254" s="49"/>
+      <c r="F254" s="2"/>
       <c r="H254" s="2"/>
     </row>
     <row r="255" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D255" s="2"/>
       <c r="E255" s="6"/>
-      <c r="F255" s="49"/>
+      <c r="F255" s="2"/>
       <c r="H255" s="2"/>
     </row>
     <row r="256" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D256" s="2"/>
       <c r="E256" s="6"/>
-      <c r="F256" s="49"/>
+      <c r="F256" s="2"/>
       <c r="H256" s="2"/>
     </row>
     <row r="257" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D257" s="2"/>
       <c r="E257" s="6"/>
-      <c r="F257" s="49"/>
+      <c r="F257" s="2"/>
       <c r="H257" s="2"/>
     </row>
     <row r="258" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D258" s="2"/>
       <c r="E258" s="6"/>
-      <c r="F258" s="49"/>
+      <c r="F258" s="2"/>
       <c r="H258" s="2"/>
     </row>
     <row r="259" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D259" s="2"/>
       <c r="E259" s="6"/>
-      <c r="F259" s="49"/>
+      <c r="F259" s="2"/>
       <c r="H259" s="2"/>
     </row>
     <row r="260" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D260" s="2"/>
       <c r="E260" s="6"/>
-      <c r="F260" s="49"/>
+      <c r="F260" s="2"/>
       <c r="H260" s="2"/>
     </row>
     <row r="261" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D261" s="2"/>
       <c r="E261" s="6"/>
-      <c r="F261" s="49"/>
+      <c r="F261" s="2"/>
       <c r="H261" s="2"/>
     </row>
     <row r="262" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D262" s="2"/>
       <c r="E262" s="6"/>
-      <c r="F262" s="49"/>
+      <c r="F262" s="2"/>
       <c r="H262" s="2"/>
     </row>
     <row r="263" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D263" s="2"/>
       <c r="E263" s="6"/>
-      <c r="F263" s="49"/>
+      <c r="F263" s="2"/>
       <c r="H263" s="2"/>
     </row>
     <row r="264" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D264" s="2"/>
       <c r="E264" s="6"/>
-      <c r="F264" s="49"/>
+      <c r="F264" s="2"/>
       <c r="H264" s="2"/>
     </row>
     <row r="265" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D265" s="2"/>
       <c r="E265" s="6"/>
-      <c r="F265" s="49"/>
+      <c r="F265" s="2"/>
       <c r="H265" s="2"/>
     </row>
     <row r="266" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D266" s="2"/>
       <c r="E266" s="6"/>
-      <c r="F266" s="49"/>
+      <c r="F266" s="2"/>
       <c r="H266" s="2"/>
     </row>
     <row r="267" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D267" s="2"/>
       <c r="E267" s="6"/>
-      <c r="F267" s="49"/>
+      <c r="F267" s="2"/>
       <c r="H267" s="2"/>
     </row>
     <row r="268" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D268" s="2"/>
       <c r="E268" s="6"/>
-      <c r="F268" s="49"/>
+      <c r="F268" s="2"/>
       <c r="H268" s="2"/>
     </row>
     <row r="269" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D269" s="2"/>
       <c r="E269" s="6"/>
-      <c r="F269" s="49"/>
+      <c r="F269" s="2"/>
       <c r="H269" s="2"/>
     </row>
     <row r="270" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D270" s="2"/>
       <c r="E270" s="6"/>
-      <c r="F270" s="49"/>
+      <c r="F270" s="2"/>
       <c r="H270" s="2"/>
     </row>
     <row r="271" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D271" s="2"/>
       <c r="E271" s="6"/>
-      <c r="F271" s="49"/>
+      <c r="F271" s="2"/>
       <c r="H271" s="2"/>
     </row>
     <row r="272" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D272" s="2"/>
       <c r="E272" s="6"/>
-      <c r="F272" s="49"/>
+      <c r="F272" s="2"/>
       <c r="H272" s="2"/>
     </row>
     <row r="273" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D273" s="2"/>
       <c r="E273" s="6"/>
-      <c r="F273" s="49"/>
+      <c r="F273" s="2"/>
       <c r="H273" s="2"/>
     </row>
     <row r="274" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D274" s="2"/>
       <c r="E274" s="6"/>
-      <c r="F274" s="49"/>
+      <c r="F274" s="2"/>
       <c r="H274" s="2"/>
     </row>
     <row r="275" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D275" s="2"/>
       <c r="E275" s="6"/>
-      <c r="F275" s="49"/>
+      <c r="F275" s="2"/>
       <c r="H275" s="2"/>
     </row>
     <row r="276" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D276" s="2"/>
       <c r="E276" s="6"/>
-      <c r="F276" s="49"/>
+      <c r="F276" s="2"/>
       <c r="H276" s="2"/>
     </row>
     <row r="277" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D277" s="2"/>
       <c r="E277" s="6"/>
-      <c r="F277" s="49"/>
+      <c r="F277" s="2"/>
       <c r="H277" s="2"/>
     </row>
     <row r="278" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D278" s="2"/>
       <c r="E278" s="6"/>
-      <c r="F278" s="49"/>
+      <c r="F278" s="2"/>
       <c r="H278" s="2"/>
     </row>
     <row r="279" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D279" s="2"/>
       <c r="E279" s="6"/>
-      <c r="F279" s="49"/>
+      <c r="F279" s="2"/>
       <c r="H279" s="2"/>
     </row>
     <row r="280" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D280" s="2"/>
       <c r="E280" s="6"/>
-      <c r="F280" s="49"/>
+      <c r="F280" s="2"/>
       <c r="H280" s="2"/>
     </row>
     <row r="281" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D281" s="2"/>
       <c r="E281" s="6"/>
-      <c r="F281" s="49"/>
+      <c r="F281" s="2"/>
       <c r="H281" s="2"/>
     </row>
     <row r="282" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D282" s="2"/>
       <c r="E282" s="6"/>
-      <c r="F282" s="49"/>
+      <c r="F282" s="2"/>
       <c r="H282" s="2"/>
     </row>
     <row r="283" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D283" s="2"/>
       <c r="E283" s="6"/>
-      <c r="F283" s="49"/>
+      <c r="F283" s="2"/>
       <c r="H283" s="2"/>
     </row>
     <row r="284" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D284" s="2"/>
       <c r="E284" s="6"/>
-      <c r="F284" s="49"/>
+      <c r="F284" s="2"/>
       <c r="H284" s="2"/>
     </row>
     <row r="285" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D285" s="2"/>
       <c r="E285" s="6"/>
-      <c r="F285" s="49"/>
+      <c r="F285" s="2"/>
       <c r="H285" s="2"/>
     </row>
     <row r="286" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D286" s="2"/>
       <c r="E286" s="6"/>
-      <c r="F286" s="49"/>
+      <c r="F286" s="2"/>
       <c r="H286" s="2"/>
     </row>
     <row r="287" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D287" s="2"/>
       <c r="E287" s="6"/>
-      <c r="F287" s="49"/>
+      <c r="F287" s="2"/>
       <c r="H287" s="2"/>
     </row>
     <row r="288" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D288" s="2"/>
       <c r="E288" s="6"/>
-      <c r="F288" s="49"/>
+      <c r="F288" s="2"/>
       <c r="H288" s="2"/>
     </row>
     <row r="289" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D289" s="2"/>
       <c r="E289" s="6"/>
-      <c r="F289" s="49"/>
+      <c r="F289" s="2"/>
       <c r="H289" s="2"/>
     </row>
     <row r="290" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D290" s="2"/>
       <c r="E290" s="6"/>
-      <c r="F290" s="49"/>
+      <c r="F290" s="2"/>
       <c r="H290" s="2"/>
     </row>
     <row r="291" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D291" s="2"/>
       <c r="E291" s="6"/>
-      <c r="F291" s="49"/>
+      <c r="F291" s="2"/>
       <c r="H291" s="2"/>
     </row>
     <row r="292" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D292" s="2"/>
       <c r="E292" s="6"/>
-      <c r="F292" s="49"/>
+      <c r="F292" s="2"/>
       <c r="H292" s="2"/>
     </row>
     <row r="293" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D293" s="2"/>
       <c r="E293" s="6"/>
-      <c r="F293" s="49"/>
+      <c r="F293" s="2"/>
       <c r="H293" s="2"/>
     </row>
     <row r="294" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D294" s="2"/>
       <c r="E294" s="6"/>
-      <c r="F294" s="49"/>
+      <c r="F294" s="2"/>
       <c r="H294" s="2"/>
     </row>
     <row r="295" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D295" s="2"/>
       <c r="E295" s="6"/>
-      <c r="F295" s="49"/>
+      <c r="F295" s="2"/>
       <c r="H295" s="2"/>
     </row>
     <row r="296" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D296" s="2"/>
       <c r="E296" s="6"/>
-      <c r="F296" s="49"/>
+      <c r="F296" s="2"/>
       <c r="H296" s="2"/>
     </row>
     <row r="297" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D297" s="2"/>
       <c r="E297" s="6"/>
-      <c r="F297" s="49"/>
+      <c r="F297" s="2"/>
       <c r="H297" s="2"/>
     </row>
     <row r="298" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D298" s="2"/>
       <c r="E298" s="6"/>
-      <c r="F298" s="49"/>
+      <c r="F298" s="2"/>
       <c r="H298" s="2"/>
     </row>
     <row r="299" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D299" s="2"/>
       <c r="E299" s="6"/>
-      <c r="F299" s="49"/>
+      <c r="F299" s="2"/>
       <c r="H299" s="2"/>
     </row>
     <row r="300" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D300" s="2"/>
       <c r="E300" s="6"/>
-      <c r="F300" s="49"/>
+      <c r="F300" s="2"/>
       <c r="H300" s="2"/>
     </row>
     <row r="301" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D301" s="2"/>
       <c r="E301" s="6"/>
-      <c r="F301" s="49"/>
+      <c r="F301" s="2"/>
       <c r="H301" s="13"/>
     </row>
     <row r="302" spans="4:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D302" s="13"/>
       <c r="E302" s="6"/>
-      <c r="F302" s="49"/>
+      <c r="F302" s="2"/>
     </row>
     <row r="1048576" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1048576" s="1"/>

</xml_diff>

<commit_message>
chore(docs): added some reqs for client side and added model process to the dependency diagram
</commit_message>
<xml_diff>
--- a/Docs/RF y RN.xlsx
+++ b/Docs/RF y RN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hecto\OneDrive\Escritorio\Personal\iroFactory\21.Mapo\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94880F9-1816-40BA-B8C6-9A74E11E1DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88334680-D6EA-4DEA-A07F-DEE608BB2748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RF-RNF" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="120">
   <si>
     <t>RF</t>
   </si>
@@ -248,9 +248,6 @@
     <t>Quizá me hace falta precisión con a qué me refiero con esto, pero realmente creo que se verá una vez entendamos cómo obtener la info de ahí</t>
   </si>
   <si>
-    <t>Django? Flask? FastAPI?</t>
-  </si>
-  <si>
     <t>Framework para integrar módulos de python</t>
   </si>
   <si>
@@ -306,6 +303,99 @@
   </si>
   <si>
     <t>Para distintos negocios se necesitan distintos valores arbitrarios iniciales</t>
+  </si>
+  <si>
+    <t>Django? Flask? FastAPI? API en js</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Necesitaríamos habilitar un enviador de correos en el dominio</t>
+  </si>
+  <si>
+    <t>Tal vez más estados para la cuenta, tipo admin o no sé</t>
+  </si>
+  <si>
+    <t>Datos sensibles</t>
+  </si>
+  <si>
+    <t>Geodata de usuario</t>
+  </si>
+  <si>
+    <t>El sistema debe clasificar al usuario, por medio del rubro, el rango de ingresos y el municipio, en una clase socioeconómica</t>
+  </si>
+  <si>
+    <t>El usuario debe poder seleccionar un rubro, un rango de ingresos y su municipio</t>
+  </si>
+  <si>
+    <t>El sistema debe registrar la fecha de creación, último acceso y estado de la cuenta (activo/inactivo)</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir a los usuarios actualizar su perfil y cambiar su contraseña</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir la recuperación de contraseña mediante correo electrónico</t>
+  </si>
+  <si>
+    <t>El sistema debe validar las credenciales ingresadas contra la base de datos de usuarios</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir a los usuarios iniciar sesión con su correo y contraseña</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir a los usuarios registrarse proporcionando nombre, correo electrónico, contraseña y rol</t>
+  </si>
+  <si>
+    <t>El sistema debe tener tolerancia y amplitud en su clusterización para el municipio/zipcode/AGEB de acuerdo a su clase socioeconómica y las zonas en las que el usuario desea analizar</t>
+  </si>
+  <si>
+    <t>Será muy invasivo que nos comparta su zipcode o ubicar su AGEB accediendo a su ubicación?</t>
+  </si>
+  <si>
+    <t>Persistencia de datos de usuario</t>
+  </si>
+  <si>
+    <t>El usuario debe poder guardar dashboards para su análisis</t>
+  </si>
+  <si>
+    <t>Cuántos dashboards? Deberíamos hacer una versión premium para tener más de dos dashboards?</t>
+  </si>
+  <si>
+    <t>A menos que alguien tenga una mejor idea</t>
+  </si>
+  <si>
+    <t>El sistema debe procesar esta información en forma de JSON y adaptarla al mapa</t>
+  </si>
+  <si>
+    <t>Los JSON deben contener georreferencias a data del servidor, y no alojar por sí mismos geodata</t>
+  </si>
+  <si>
+    <t>Los ítems deben tener referencias a la información que muestran</t>
+  </si>
+  <si>
+    <t>Los ítems deben tener tipo de gráfica que muestra la información a la que hacen referencia</t>
+  </si>
+  <si>
+    <t>Los ítems deben tener metadata de altura, ancho y posición en el dashboard</t>
+  </si>
+  <si>
+    <t>Los dashboards son como canvas que contienen ítems</t>
+  </si>
+  <si>
+    <t>Los ítems se guardan con un ID único en su propia tabla</t>
+  </si>
+  <si>
+    <t>Los dashboards se guardan con un ID único en su propia tabla</t>
+  </si>
+  <si>
+    <t>Dashboards</t>
+  </si>
+  <si>
+    <t>Ítems de dashboards</t>
+  </si>
+  <si>
+    <t>Cifrar las contraseñas de usuario con hashing</t>
   </si>
 </sst>
 </file>
@@ -397,7 +487,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="62">
+  <fills count="73">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -762,6 +852,72 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor rgb="FFFFE599"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor rgb="FFFFE599"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor rgb="FF93C47D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor rgb="FF93C47D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor rgb="FF6AA84F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor rgb="FF38761D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor rgb="FFDD7E6B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor rgb="FF6AA84F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor rgb="FF6AA84F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor rgb="FF6AA84F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor rgb="FF38761D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor rgb="FF38761D"/>
       </patternFill>
     </fill>
   </fills>
@@ -814,7 +970,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -929,12 +1085,6 @@
     <xf numFmtId="0" fontId="2" fillId="53" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="54" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -959,9 +1109,6 @@
     <xf numFmtId="0" fontId="5" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -998,16 +1145,7 @@
     <xf numFmtId="0" fontId="8" fillId="59" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="60" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1015,6 +1153,39 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="61" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="62" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="63" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="66" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="65" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="64" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="67" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="68" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="69" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="70" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="71" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="72" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1245,8 +1416,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1263,33 +1434,33 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9">
-        <v>45848</v>
+        <v>45855</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="80" t="s">
+      <c r="C2" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="81" t="s">
+      <c r="D2" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="81" t="s">
+      <c r="E2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="82" t="s">
+      <c r="F2" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="80" t="s">
+      <c r="G2" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="82" t="s">
+      <c r="H2" s="79" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1340,10 +1511,10 @@
         <v>33</v>
       </c>
       <c r="H4" s="47" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A5" s="48">
         <v>3</v>
       </c>
@@ -1359,17 +1530,13 @@
       <c r="E5" s="48">
         <v>3</v>
       </c>
-      <c r="F5" s="50" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="53" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="47" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="66" x14ac:dyDescent="0.25">
+      <c r="F5" s="47"/>
+      <c r="G5" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="H5" s="47"/>
+    </row>
+    <row r="6" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A6" s="48">
         <v>4</v>
       </c>
@@ -1384,13 +1551,13 @@
         <v>4</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="56" t="s">
-        <v>46</v>
+        <v>36</v>
+      </c>
+      <c r="G6" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="47" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="66" x14ac:dyDescent="0.25">
@@ -1408,13 +1575,13 @@
         <v>5</v>
       </c>
       <c r="F7" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="59" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="47" t="s">
-        <v>47</v>
+        <v>37</v>
+      </c>
+      <c r="G7" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="56" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="66" x14ac:dyDescent="0.25">
@@ -1432,14 +1599,16 @@
         <v>6</v>
       </c>
       <c r="F8" s="50" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G8" s="59" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="50"/>
-    </row>
-    <row r="9" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="H8" s="47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A9" s="48">
         <v>7</v>
       </c>
@@ -1454,10 +1623,10 @@
         <v>7</v>
       </c>
       <c r="F9" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="62" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+      <c r="G9" s="59" t="s">
+        <v>42</v>
       </c>
       <c r="H9" s="50"/>
     </row>
@@ -1477,11 +1646,11 @@
       <c r="E10" s="48">
         <v>8</v>
       </c>
-      <c r="F10" s="47" t="s">
-        <v>65</v>
-      </c>
-      <c r="G10" s="50" t="s">
-        <v>66</v>
+      <c r="F10" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="62" t="s">
+        <v>44</v>
       </c>
       <c r="H10" s="50"/>
     </row>
@@ -1499,9 +1668,11 @@
       <c r="E11" s="48">
         <v>9</v>
       </c>
-      <c r="F11" s="50"/>
+      <c r="F11" s="47" t="s">
+        <v>65</v>
+      </c>
       <c r="G11" s="50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H11" s="50"/>
     </row>
@@ -1521,15 +1692,13 @@
       <c r="E12" s="48">
         <v>10</v>
       </c>
-      <c r="F12" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" s="89" t="s">
-        <v>73</v>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50" t="s">
+        <v>67</v>
       </c>
       <c r="H12" s="50"/>
     </row>
-    <row r="13" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A13" s="57">
         <v>11</v>
       </c>
@@ -1546,14 +1715,12 @@
         <v>11</v>
       </c>
       <c r="F13" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="93" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" s="47" t="s">
-        <v>75</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="G13" s="86" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="50"/>
     </row>
     <row r="14" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A14" s="48">
@@ -1568,10 +1735,18 @@
       <c r="D14" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="48"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="69"/>
+      <c r="E14" s="48">
+        <v>12</v>
+      </c>
+      <c r="F14" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="88" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="47" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A15" s="48">
@@ -1580,13 +1755,15 @@
       <c r="B15" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="70" t="s">
+      <c r="C15" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="84"/>
-      <c r="E15" s="48"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="48">
+        <v>13</v>
+      </c>
       <c r="F15" s="50"/>
-      <c r="G15" s="71"/>
+      <c r="G15" s="69"/>
       <c r="H15" s="50"/>
     </row>
     <row r="16" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
@@ -1596,13 +1773,15 @@
       <c r="B16" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="72" t="s">
+      <c r="C16" s="70" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="50"/>
-      <c r="E16" s="48"/>
+      <c r="E16" s="48">
+        <v>14</v>
+      </c>
       <c r="F16" s="50"/>
-      <c r="G16" s="73"/>
+      <c r="G16" s="71"/>
       <c r="H16" s="50"/>
     </row>
     <row r="17" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
@@ -1612,15 +1791,17 @@
       <c r="B17" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="85" t="s">
-        <v>78</v>
+      <c r="C17" s="82" t="s">
+        <v>77</v>
       </c>
       <c r="D17" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="48"/>
+      <c r="E17" s="48">
+        <v>15</v>
+      </c>
       <c r="F17" s="50"/>
-      <c r="G17" s="73"/>
+      <c r="G17" s="71"/>
       <c r="H17" s="50"/>
     </row>
     <row r="18" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
@@ -1628,13 +1809,15 @@
         <v>16</v>
       </c>
       <c r="B18" s="50"/>
-      <c r="C18" s="85" t="s">
-        <v>79</v>
+      <c r="C18" s="82" t="s">
+        <v>78</v>
       </c>
       <c r="D18" s="50"/>
-      <c r="E18" s="48"/>
+      <c r="E18" s="48">
+        <v>16</v>
+      </c>
       <c r="F18" s="50"/>
-      <c r="G18" s="74"/>
+      <c r="G18" s="72"/>
       <c r="H18" s="50"/>
     </row>
     <row r="19" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
@@ -1642,13 +1825,15 @@
         <v>17</v>
       </c>
       <c r="B19" s="50"/>
-      <c r="C19" s="85" t="s">
-        <v>82</v>
+      <c r="C19" s="82" t="s">
+        <v>81</v>
       </c>
       <c r="D19" s="50"/>
-      <c r="E19" s="48"/>
+      <c r="E19" s="48">
+        <v>17</v>
+      </c>
       <c r="F19" s="50"/>
-      <c r="G19" s="74"/>
+      <c r="G19" s="72"/>
       <c r="H19" s="50"/>
     </row>
     <row r="20" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
@@ -1656,65 +1841,71 @@
         <v>18</v>
       </c>
       <c r="B20" s="50"/>
-      <c r="C20" s="85" t="s">
+      <c r="C20" s="82" t="s">
         <v>59</v>
       </c>
       <c r="D20" s="50"/>
-      <c r="E20" s="48"/>
+      <c r="E20" s="48">
+        <v>18</v>
+      </c>
       <c r="F20" s="50"/>
-      <c r="G20" s="74"/>
+      <c r="G20" s="72"/>
       <c r="H20" s="50"/>
     </row>
     <row r="21" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A21" s="48">
         <v>19</v>
       </c>
-      <c r="B21" s="87" t="s">
+      <c r="B21" s="84" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="86" t="s">
+      <c r="C21" s="83" t="s">
         <v>68</v>
       </c>
       <c r="D21" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="48"/>
+      <c r="E21" s="48">
+        <v>19</v>
+      </c>
       <c r="F21" s="50"/>
-      <c r="G21" s="74"/>
+      <c r="G21" s="72"/>
       <c r="H21" s="50"/>
     </row>
-    <row r="22" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A22" s="48">
         <v>20</v>
       </c>
-      <c r="B22" s="87"/>
-      <c r="C22" s="86" t="s">
-        <v>71</v>
+      <c r="B22" s="84"/>
+      <c r="C22" s="83" t="s">
+        <v>70</v>
       </c>
       <c r="D22" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="48"/>
+        <v>89</v>
+      </c>
+      <c r="E22" s="48">
+        <v>20</v>
+      </c>
       <c r="F22" s="50"/>
-      <c r="G22" s="75"/>
+      <c r="G22" s="73"/>
       <c r="H22" s="50"/>
     </row>
     <row r="23" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A23" s="48">
         <v>21</v>
       </c>
-      <c r="B23" s="87" t="s">
+      <c r="B23" s="84" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="88" t="s">
-        <v>76</v>
+      <c r="C23" s="85" t="s">
+        <v>75</v>
       </c>
       <c r="D23" s="50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E23" s="48"/>
       <c r="F23" s="50"/>
-      <c r="G23" s="76"/>
+      <c r="G23" s="74"/>
       <c r="H23" s="50"/>
     </row>
     <row r="24" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
@@ -1724,15 +1915,15 @@
       <c r="B24" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="95" t="s">
-        <v>77</v>
+      <c r="C24" s="89" t="s">
+        <v>76</v>
       </c>
       <c r="D24" s="47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E24" s="48"/>
       <c r="F24" s="50"/>
-      <c r="G24" s="76"/>
+      <c r="G24" s="74"/>
       <c r="H24" s="50"/>
     </row>
     <row r="25" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -1740,17 +1931,17 @@
         <v>23</v>
       </c>
       <c r="B25" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="90" t="s">
         <v>84</v>
       </c>
+      <c r="C25" s="87" t="s">
+        <v>83</v>
+      </c>
       <c r="D25" s="47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E25" s="48"/>
       <c r="F25" s="50"/>
-      <c r="G25" s="77"/>
+      <c r="G25" s="75"/>
       <c r="H25" s="50"/>
     </row>
     <row r="26" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
@@ -1758,15 +1949,15 @@
         <v>24</v>
       </c>
       <c r="B26" s="47"/>
-      <c r="C26" s="90" t="s">
+      <c r="C26" s="87" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="47" t="s">
         <v>86</v>
-      </c>
-      <c r="D26" s="47" t="s">
-        <v>87</v>
       </c>
       <c r="E26" s="48"/>
       <c r="F26" s="50"/>
-      <c r="G26" s="76"/>
+      <c r="G26" s="74"/>
       <c r="H26" s="50"/>
     </row>
     <row r="27" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
@@ -1774,10 +1965,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="91" t="s">
         <v>88</v>
-      </c>
-      <c r="C27" s="97" t="s">
-        <v>89</v>
       </c>
       <c r="D27" s="50"/>
       <c r="E27" s="6"/>
@@ -1785,181 +1976,275 @@
       <c r="G27" s="21"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="50"/>
-      <c r="C28" s="78"/>
+    <row r="28" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A28" s="48">
+        <v>26</v>
+      </c>
+      <c r="B28" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="92" t="s">
+        <v>102</v>
+      </c>
       <c r="D28" s="50"/>
       <c r="E28" s="6"/>
       <c r="F28" s="2"/>
       <c r="G28" s="21"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
+    <row r="29" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A29" s="48">
+        <v>27</v>
+      </c>
       <c r="B29" s="47"/>
-      <c r="C29" s="59"/>
+      <c r="C29" s="93" t="s">
+        <v>101</v>
+      </c>
       <c r="D29" s="50"/>
       <c r="E29" s="6"/>
       <c r="F29" s="2"/>
       <c r="G29" s="14"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
+    <row r="30" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A30" s="48">
+        <v>28</v>
+      </c>
       <c r="B30" s="47"/>
-      <c r="C30" s="68"/>
+      <c r="C30" s="93" t="s">
+        <v>100</v>
+      </c>
       <c r="D30" s="50"/>
       <c r="E30" s="6"/>
       <c r="F30" s="2"/>
       <c r="G30" s="14"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="50"/>
-      <c r="C31" s="68"/>
-      <c r="D31" s="50"/>
+    <row r="31" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>29</v>
+      </c>
+      <c r="B31" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="96" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" s="50" t="s">
+        <v>91</v>
+      </c>
       <c r="E31" s="6"/>
       <c r="F31" s="2"/>
       <c r="G31" s="14"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
+    <row r="32" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A32" s="48">
+        <v>30</v>
+      </c>
       <c r="B32" s="50"/>
-      <c r="C32" s="68"/>
+      <c r="C32" s="95" t="s">
+        <v>98</v>
+      </c>
       <c r="D32" s="50"/>
       <c r="E32" s="6"/>
       <c r="F32" s="2"/>
       <c r="G32" s="14"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
+    <row r="33" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A33" s="48">
+        <v>31</v>
+      </c>
       <c r="B33" s="50"/>
-      <c r="C33" s="91"/>
-      <c r="D33" s="50"/>
+      <c r="C33" s="94" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" s="50" t="s">
+        <v>92</v>
+      </c>
       <c r="E33" s="6"/>
       <c r="F33" s="2"/>
       <c r="G33" s="14"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="50"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="50"/>
+    <row r="34" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A34" s="48">
+        <v>32</v>
+      </c>
+      <c r="B34" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="97" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" s="47" t="s">
+        <v>104</v>
+      </c>
       <c r="E34" s="6"/>
       <c r="F34" s="2"/>
       <c r="G34" s="22"/>
       <c r="H34" s="2"/>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
+    <row r="35" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
+        <v>33</v>
+      </c>
       <c r="B35" s="50"/>
-      <c r="C35" s="94"/>
+      <c r="C35" s="98" t="s">
+        <v>95</v>
+      </c>
       <c r="D35" s="50"/>
       <c r="E35" s="6"/>
       <c r="F35" s="2"/>
       <c r="G35" s="22"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
+    <row r="36" spans="1:9" ht="66" x14ac:dyDescent="0.25">
+      <c r="A36" s="48">
+        <v>34</v>
+      </c>
       <c r="B36" s="50"/>
-      <c r="C36" s="62"/>
+      <c r="C36" s="98" t="s">
+        <v>103</v>
+      </c>
       <c r="D36" s="50"/>
       <c r="E36" s="6"/>
       <c r="F36" s="2"/>
       <c r="G36" s="22"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="47"/>
-      <c r="C37" s="62"/>
-      <c r="D37" s="50"/>
+    <row r="37" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A37" s="48">
+        <v>35</v>
+      </c>
+      <c r="B37" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" s="99" t="s">
+        <v>106</v>
+      </c>
+      <c r="D37" s="47" t="s">
+        <v>107</v>
+      </c>
       <c r="E37" s="6"/>
       <c r="F37" s="2"/>
       <c r="G37" s="22"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
+    <row r="38" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A38" s="48">
+        <v>36</v>
+      </c>
       <c r="B38" s="50"/>
-      <c r="C38" s="62"/>
-      <c r="D38" s="50"/>
+      <c r="C38" s="99" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" s="47" t="s">
+        <v>108</v>
+      </c>
       <c r="E38" s="6"/>
       <c r="F38" s="2"/>
       <c r="G38" s="22"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
+    <row r="39" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A39" s="6">
+        <v>37</v>
+      </c>
       <c r="B39" s="50"/>
-      <c r="C39" s="92"/>
+      <c r="C39" s="99" t="s">
+        <v>110</v>
+      </c>
       <c r="D39" s="50"/>
       <c r="E39" s="6"/>
       <c r="F39" s="2"/>
       <c r="G39" s="23"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="50"/>
-      <c r="C40" s="92"/>
+    <row r="40" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A40" s="48">
+        <v>38</v>
+      </c>
+      <c r="B40" s="47" t="s">
+        <v>117</v>
+      </c>
+      <c r="C40" s="100" t="s">
+        <v>116</v>
+      </c>
       <c r="D40" s="50"/>
       <c r="E40" s="6"/>
       <c r="F40" s="2"/>
       <c r="G40" s="23"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
+    <row r="41" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A41" s="48">
+        <v>39</v>
+      </c>
       <c r="B41" s="47"/>
-      <c r="C41" s="92"/>
+      <c r="C41" s="101" t="s">
+        <v>114</v>
+      </c>
       <c r="D41" s="50"/>
       <c r="E41" s="6"/>
       <c r="F41" s="2"/>
       <c r="G41" s="23"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="B42" s="50"/>
-      <c r="C42" s="92"/>
+    <row r="42" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A42" s="48">
+        <v>40</v>
+      </c>
+      <c r="B42" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" s="102" t="s">
+        <v>115</v>
+      </c>
       <c r="D42" s="50"/>
       <c r="E42" s="6"/>
       <c r="F42" s="2"/>
       <c r="G42" s="23"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
+    <row r="43" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>41</v>
+      </c>
       <c r="B43" s="50"/>
-      <c r="C43" s="92"/>
+      <c r="C43" s="102" t="s">
+        <v>111</v>
+      </c>
       <c r="D43" s="50"/>
       <c r="E43" s="6"/>
       <c r="F43" s="2"/>
       <c r="G43" s="23"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
+    <row r="44" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A44" s="48">
+        <v>42</v>
+      </c>
       <c r="B44" s="50"/>
-      <c r="C44" s="92"/>
+      <c r="C44" s="102" t="s">
+        <v>112</v>
+      </c>
       <c r="D44" s="50"/>
       <c r="E44" s="6"/>
       <c r="F44" s="2"/>
       <c r="G44" s="23"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
+    <row r="45" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A45" s="48">
+        <v>43</v>
+      </c>
       <c r="B45" s="8"/>
-      <c r="C45" s="15"/>
+      <c r="C45" s="102" t="s">
+        <v>113</v>
+      </c>
       <c r="D45" s="50"/>
       <c r="E45" s="6"/>
       <c r="F45" s="2"/>
@@ -1967,7 +2252,9 @@
       <c r="H45" s="2"/>
     </row>
     <row r="46" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
+      <c r="A46" s="48">
+        <v>44</v>
+      </c>
       <c r="B46" s="2"/>
       <c r="C46" s="15"/>
       <c r="D46" s="50"/>
@@ -1977,7 +2264,9 @@
       <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
+      <c r="A47" s="6">
+        <v>45</v>
+      </c>
       <c r="B47" s="2"/>
       <c r="C47" s="15"/>
       <c r="D47" s="50"/>
@@ -1987,7 +2276,9 @@
       <c r="H47" s="2"/>
     </row>
     <row r="48" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
+      <c r="A48" s="48">
+        <v>46</v>
+      </c>
       <c r="B48" s="8"/>
       <c r="C48" s="24"/>
       <c r="D48" s="50"/>
@@ -1997,9 +2288,11 @@
       <c r="H48" s="2"/>
     </row>
     <row r="49" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
+      <c r="A49" s="48">
+        <v>47</v>
+      </c>
       <c r="B49" s="2"/>
-      <c r="C49" s="96"/>
+      <c r="C49" s="90"/>
       <c r="D49" s="50"/>
       <c r="E49" s="6"/>
       <c r="F49" s="2"/>
@@ -2007,7 +2300,9 @@
       <c r="H49" s="2"/>
     </row>
     <row r="50" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
+      <c r="A50" s="48">
+        <v>48</v>
+      </c>
       <c r="B50" s="2"/>
       <c r="C50" s="19"/>
       <c r="D50" s="50"/>
@@ -2017,7 +2312,9 @@
       <c r="H50" s="2"/>
     </row>
     <row r="51" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
+      <c r="A51" s="6">
+        <v>49</v>
+      </c>
       <c r="B51" s="8"/>
       <c r="C51" s="19"/>
       <c r="D51" s="50"/>
@@ -2027,9 +2324,11 @@
       <c r="H51" s="2"/>
     </row>
     <row r="52" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A52" s="6"/>
+      <c r="A52" s="48">
+        <v>50</v>
+      </c>
       <c r="B52" s="2"/>
-      <c r="C52" s="96"/>
+      <c r="C52" s="90"/>
       <c r="D52" s="50"/>
       <c r="E52" s="6"/>
       <c r="F52" s="2"/>

</xml_diff>